<commit_message>
feat:role trans data, but not imp full dec
</commit_message>
<xml_diff>
--- a/ExtremeRolesTransData.xlsx
+++ b/ExtremeRolesTransData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ドキュメント\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1988829-5BA6-40F7-AA8F-D0899E89C0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A813793-7FD9-43CF-9ED2-3492279BD19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1428" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1621" uniqueCount="1329">
   <si>
     <t>English</t>
   </si>
@@ -8772,12 +8772,661 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>JesterUseSabotage</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ジェスターがサボタージュを使えるか</t>
+    <rPh sb="13" eb="14">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>YandereRoleNum</t>
+  </si>
+  <si>
+    <t>YandereHasOtherVison</t>
+  </si>
+  <si>
+    <t>YandereVison</t>
+  </si>
+  <si>
+    <t>YandereApplyEnvironmentVisionEffect</t>
+  </si>
+  <si>
+    <t>YandereTargetKilledKillCoolReduceRate</t>
+  </si>
+  <si>
+    <t>YandereNoneTargetKilledKillCoolMultiplier</t>
+  </si>
+  <si>
+    <t>YandereSetTargetRange</t>
+  </si>
+  <si>
+    <t>YandereSetTargetTime</t>
+  </si>
+  <si>
+    <t>YandereMaxTargetNum</t>
+  </si>
+  <si>
+    <t>YandereRunawayTime</t>
+  </si>
+  <si>
+    <t>YandereHasOneSidedArrow</t>
+  </si>
+  <si>
+    <t>YandereSpawnRate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yandere</t>
+  </si>
+  <si>
+    <t>ヤンデレ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「邪魔者」を殺した時のキルクール減少率</t>
+    <rPh sb="1" eb="4">
+      <t>ジャマモノ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>コロ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="18" eb="19">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「邪魔者」以外を殺したときのキルクールペナルティ</t>
+    <rPh sb="1" eb="4">
+      <t>ジャマモノ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>コロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「邪魔者」が登録される「片思いの人」からの距離</t>
+    <rPh sb="6" eb="8">
+      <t>トウロク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>カタオモ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>ヒト</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>キョリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「邪魔者」が登録される時間</t>
+    <rPh sb="1" eb="3">
+      <t>カタ_x0000__x0001_</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「片思いの人」を指す矢印を表示するか</t>
+    <rPh sb="8" eb="9">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヤジルシ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「邪魔者」を指す矢印を表示するか</t>
+    <rPh sb="1" eb="4">
+      <t>ジャマモノ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヤジルシ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「邪魔者」の登録数上限</t>
+    <rPh sb="1" eb="3">
+      <t>カタ_x0000__x0001_</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>_x0002__x0004_</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「邪魔者」が無くなってから「暴走」するまでの時間</t>
+    <rPh sb="1" eb="4">
+      <t>ジャマモノ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ナ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ボウソウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>YandereHasTargetArrow</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>YandereIntroDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>YandereShortDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>YandereFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「{0}」は私のもの</t>
+    <rPh sb="6" eb="7">
+      <t>ワタシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「{0}」に近づく恋敵を皆殺しにしろ</t>
+    <rPh sb="6" eb="8">
+      <t>チカズ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>コイガタキ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ミナゴロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>YandereShipJustForTwo</t>
+  </si>
+  <si>
+    <t>ヤンデレの恋が成熟した</t>
+    <rPh sb="5" eb="6">
+      <t>コイ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>セイジュク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LoverBecomeNeutralLoverHasOtherVison</t>
+  </si>
+  <si>
+    <t>LoverBecomeNeutralLoverVison</t>
+  </si>
+  <si>
+    <t>LoverBecomeNeutralLoverApplyEnvironmentVisionEffect</t>
+  </si>
+  <si>
+    <t>LoverBecomeNeutralLoverCanUseVent</t>
+  </si>
+  <si>
+    <t>第三陣営に変化後、別の視界設定を持つか</t>
+    <rPh sb="5" eb="7">
+      <t>ヘンカ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ゴ</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>ベツ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>シカイ</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>セッテイ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>モ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第三陣営に変化後のビジョン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第三陣営に変化後、視界効果を受けるか</t>
+    <rPh sb="9" eb="11">
+      <t>シカイ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>コウカ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>ウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>第三陣営に変化後、ベントを使用できるか</t>
+    <rPh sb="13" eb="15">
+      <t>シヨウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SlaveDriverRoleNum</t>
+  </si>
+  <si>
+    <t>SlaveDriverHasOtherVison</t>
+  </si>
+  <si>
+    <t>SlaveDriverVison</t>
+  </si>
+  <si>
+    <t>SlaveDriverApplyEnvironmentVisionEffect</t>
+  </si>
+  <si>
+    <t>SlaveDriverHasOtherKillCool</t>
+  </si>
+  <si>
+    <t>SlaveDriverKillCoolDown</t>
+  </si>
+  <si>
+    <t>SlaveDriverHasOtherKillRange</t>
+  </si>
+  <si>
+    <t>SlaveDriverKillRange</t>
+  </si>
+  <si>
+    <t>SlaveDriverTaskProgressRange</t>
+  </si>
+  <si>
+    <t>SlaveDriverKillCoolReduceRate</t>
+  </si>
+  <si>
+    <t>SlaveDriverSpecialAttackTimer</t>
+  </si>
+  <si>
+    <t>SlaveDriverSpecialAttackAliveTimer</t>
+  </si>
+  <si>
+    <t>SlaveDriverSpecialAttackKillCoolReduceRate</t>
+  </si>
+  <si>
+    <t>SlaveDriverNoneTaskPlayerAttakBonusChance</t>
+  </si>
+  <si>
+    <t>SlaveDriverNoneTaskPlayerSpecialAttackChance</t>
+  </si>
+  <si>
+    <t>SlaveDriverAdditionalCommonTaskNum</t>
+  </si>
+  <si>
+    <t>SlaveDriverAdditionalNormalTaskNum</t>
+  </si>
+  <si>
+    <t>SlaveDriverSpawnRate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SlaveDriver</t>
+  </si>
+  <si>
+    <t>スレイヴドライバー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>生存者とタスク進捗による「特攻」が入るようになる時間</t>
+    <rPh sb="0" eb="3">
+      <t>セイゾンシャ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>シンチョク</t>
+    </rPh>
+    <rPh sb="13" eb="15">
+      <t>トッコウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ゲーム開始から「特攻」が入らない時間</t>
+    <rPh sb="3" eb="5">
+      <t>カイシ</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「特攻」が入った時のキルクール減少率</t>
+    <rPh sb="1" eb="3">
+      <t>トッコウ</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ハイ</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>トキ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キルクール減少が入らない全体のタスク進捗からの誤差</t>
+    <rPh sb="12" eb="14">
+      <t>ゼンタイ</t>
+    </rPh>
+    <rPh sb="23" eb="25">
+      <t>ゴサ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「特攻」で追加されるコモンタスクの数</t>
+    <rPh sb="1" eb="3">
+      <t>トッコウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>カズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「特攻」で追加される通常タスクの数</t>
+    <rPh sb="1" eb="3">
+      <t>トッコウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ツウジョウ</t>
+    </rPh>
+    <rPh sb="16" eb="17">
+      <t>カズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「特攻」で追加されるロングタスクの数</t>
+    <rPh sb="1" eb="3">
+      <t>トッコウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ツイカ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>カズ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SlaveDriverAdditionalLongTaskNum</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SlaveDriverIntroDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SlaveDriverShortDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SlaveDriverFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SandWormRoleNum</t>
+  </si>
+  <si>
+    <t>SandWormHasOtherVison</t>
+  </si>
+  <si>
+    <t>SandWormVison</t>
+  </si>
+  <si>
+    <t>SandWormApplyEnvironmentVisionEffect</t>
+  </si>
+  <si>
+    <t>SandWormHasOtherKillCool</t>
+  </si>
+  <si>
+    <t>SandWormKillCoolDown</t>
+  </si>
+  <si>
+    <t>SandWormHasOtherKillRange</t>
+  </si>
+  <si>
+    <t>SandWormKillRange</t>
+  </si>
+  <si>
+    <t>SandWormKillCoolPenalty</t>
+  </si>
+  <si>
+    <t>SandWormAssaultKillCoolReduce</t>
+  </si>
+  <si>
+    <t>SandWormAssaultRange</t>
+  </si>
+  <si>
+    <t>SandWormAbilityCoolTime</t>
+  </si>
+  <si>
+    <t>SandWormSpawnRate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SandWorm</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サンドワーム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タスクを持たない船員をキルしたときの「特攻」発生の確率</t>
+    <rPh sb="4" eb="5">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>センイン</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>トッコウ</t>
+    </rPh>
+    <rPh sb="22" eb="24">
+      <t>ハッセイ</t>
+    </rPh>
+    <rPh sb="25" eb="27">
+      <t>カクリツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タスクを持たない船員をキルしたときの「ボーナス」発生の確率</t>
+    <rPh sb="4" eb="5">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>センイン</t>
+    </rPh>
+    <rPh sb="24" eb="26">
+      <t>ハッセイ</t>
+    </rPh>
+    <rPh sb="27" eb="29">
+      <t>カクリツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「ボーナス」のキルクール減少率</t>
+    <rPh sb="14" eb="15">
+      <t>リツ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>サボってるクルーのケツに火をつけろ</t>
+    <rPh sb="12" eb="13">
+      <t>ヒ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>通常キルのキルクールペナルティ</t>
+    <rPh sb="0" eb="2">
+      <t>ツウジョウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「強襲」使用時のキルクールボーナス</t>
+    <rPh sb="1" eb="3">
+      <t>キョウシュウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「強襲」が使用できる範囲</t>
+    <rPh sb="1" eb="3">
+      <t>キョウシュウ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ハンイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「強襲」のクールタイム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SandWormIntroDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SandWormShortDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>光が苦手で暗闇が大好なインポスター</t>
+    <rPh sb="0" eb="1">
+      <t>ヒカリ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ニガテ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>クラヤミ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ダイス</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ベントからの「強襲」使いこなせ</t>
+    <rPh sb="7" eb="9">
+      <t>キョウシュウ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>assault</t>
+  </si>
+  <si>
+    <t>強襲</t>
+    <rPh sb="0" eb="2">
+      <t>キョウシュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>仕事をやらないクルーを粛清せよ</t>
+    <rPh sb="0" eb="2">
+      <t>シゴト</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BakaryGoodBakeTime</t>
+  </si>
+  <si>
+    <t>BakaryBadBakeTime</t>
+  </si>
+  <si>
+    <t>パンが焦げる会議との合間時間</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>パンが焼ける会議との合間時間</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>会議毎にパンが焼けたことを報告するクルー役職
 死亡するまでひたすらパンが焼けてることを報告します
 パン屋の役職が変化してもパンを焼き続けます
 パンの焼き加減が変わる場合、以下の秒数で焼き加減が変化する
-　・「パンが焼けない会議との合間時間」以下：生焼け
-　・「パンが焼けない会議との合間時間」以上～「パンが焦げる
+　・「パンが焼ける会議との合間時間」以下：生焼け
+　・「パンが焼ける会議との合間時間」以上～「パンが焦げる
 　　会議との合間時間」：美味しいパン
 　・それ以外：焦げパン</t>
     <rPh sb="0" eb="2">
@@ -8837,32 +9486,347 @@
     <rPh sb="96" eb="98">
       <t>ヘンカ</t>
     </rPh>
-    <rPh sb="107" eb="108">
-      <t>ヤ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
+    <rPh sb="119" eb="121">
+      <t>ナマヤ</t>
+    </rPh>
+    <rPh sb="125" eb="127">
       <t>カイギ</t>
     </rPh>
-    <rPh sb="115" eb="117">
-      <t>アイマ</t>
-    </rPh>
-    <rPh sb="117" eb="119">
+    <rPh sb="151" eb="152">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="179" eb="181">
+      <t>イガイ</t>
+    </rPh>
+    <rPh sb="182" eb="183">
+      <t>コ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CurseMakerRoleNum</t>
+  </si>
+  <si>
+    <t>CurseMakerHasOtherVison</t>
+  </si>
+  <si>
+    <t>CurseMakerVison</t>
+  </si>
+  <si>
+    <t>CurseMakerApplyEnvironmentVisionEffect</t>
+  </si>
+  <si>
+    <t>CurseMakerCursingRange</t>
+  </si>
+  <si>
+    <t>CurseMakerAdditionalKillCool</t>
+  </si>
+  <si>
+    <t>CurseMakerAbilityCoolTime</t>
+  </si>
+  <si>
+    <t>CurseMakerAbilityActiveTime</t>
+  </si>
+  <si>
+    <t>CurseMakerAbilityCount</t>
+  </si>
+  <si>
+    <t>CurseMakerSpawnRate</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CurseMaker</t>
+  </si>
+  <si>
+    <t>カースメーカー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「呪い」が発動できる死体からの距離</t>
+    <rPh sb="1" eb="2">
+      <t>ノロ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ハツドウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>キョリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「呪い」によって付与されるキルクールペナルティ</t>
+    <rPh sb="1" eb="2">
+      <t>ノロ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>フヨ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「呪い」のクールタイム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「呪い」の使用回数</t>
+    <rPh sb="5" eb="7">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>カイスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「呪い」が完了するまでの時間</t>
+    <rPh sb="1" eb="2">
+      <t>ノロ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>カンリョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
       <t>ジカン</t>
     </rPh>
-    <rPh sb="120" eb="122">
-      <t>ナマヤ</t>
-    </rPh>
-    <rPh sb="126" eb="128">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="153" eb="154">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="181" eb="183">
-      <t>イガイ</t>
-    </rPh>
-    <rPh sb="184" eb="185">
-      <t>コ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>死体を指す矢印を表示するか</t>
+    <rPh sb="0" eb="2">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>サ</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>ヤジルシ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヒョウジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キルされてから矢印が表示されるまでの時間</t>
+    <rPh sb="7" eb="9">
+      <t>ヤジルシ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ヒョウジ</t>
+    </rPh>
+    <rPh sb="18" eb="20">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CurseMakerIsDeadBodySearch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CurseMakerIsMultiDeadBodySearch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FencerSpawnRate</t>
+  </si>
+  <si>
+    <t>FencerRoleNum</t>
+  </si>
+  <si>
+    <t>FencerHasOtherVison</t>
+  </si>
+  <si>
+    <t>FencerVison</t>
+  </si>
+  <si>
+    <t>FencerApplyEnvironmentVisionEffect</t>
+  </si>
+  <si>
+    <t>FencerResetTime</t>
+  </si>
+  <si>
+    <t>FencerAbilityCoolTime</t>
+  </si>
+  <si>
+    <t>FencerAbilityActiveTime</t>
+  </si>
+  <si>
+    <t>Fencer</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>フェンサー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キルが付与されてからなくなるまでの時間</t>
+    <rPh sb="3" eb="5">
+      <t>フヨ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「カウンター」のクールタイム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「カウンター」の受付時間</t>
+    <rPh sb="8" eb="12">
+      <t>ウケツケジカン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「カウンター」の使用回数</t>
+    <rPh sb="8" eb="10">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>カイスウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CurseMakerSearchDeadBodyTime</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CurseMakerIntroDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CurseMakerShortDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CurseMakerFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>死体の怨念から殺した相手を呪え</t>
+    <rPh sb="0" eb="2">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>オンネン</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>コロ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>アイテ</t>
+    </rPh>
+    <rPh sb="13" eb="14">
+      <t>ノロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>怨念の恨みを果たせ</t>
+    <rPh sb="0" eb="2">
+      <t>オンネン</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>ウラ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>ハ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>curse</t>
+  </si>
+  <si>
+    <t>呪い</t>
+    <rPh sb="0" eb="1">
+      <t>ノロ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>cursing</t>
+  </si>
+  <si>
+    <t>呪術中</t>
+    <rPh sb="0" eb="2">
+      <t>ジュジュツ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>チュウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>counter</t>
+  </si>
+  <si>
+    <t>カウンター</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FencerAbilityCount</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FencerIntroDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FencerShortDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FencerFullDescription</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>「カウンター」でキルしてきた相手を返り討ちにしろ</t>
+    <rPh sb="14" eb="16">
+      <t>アイテ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>カエ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>ウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キルしてきた相手を「カウンター」で切り返せ</t>
+    <rPh sb="6" eb="8">
+      <t>アイテ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>キ</t>
+    </rPh>
+    <rPh sb="19" eb="20">
+      <t>カエ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>複数回、死体への矢印を表示させるか</t>
+    <rPh sb="0" eb="3">
+      <t>フクスウカイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>シタイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヤジルシ</t>
+    </rPh>
+    <rPh sb="11" eb="13">
+      <t>ヒョウジ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -8871,7 +9835,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -8883,6 +9847,13 @@
       <sz val="6"/>
       <name val="游ゴシック"/>
       <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -9197,8 +10168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q168"/>
   <sheetViews>
-    <sheetView topLeftCell="C114" workbookViewId="0">
-      <selection activeCell="M50" sqref="M50"/>
+    <sheetView topLeftCell="A120" workbookViewId="0">
+      <selection activeCell="B131" sqref="B131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -10435,10 +11406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
-  <dimension ref="A1:Q159"/>
+  <dimension ref="A1:Q196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B171" sqref="B171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -11620,51 +12591,325 @@
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A154" t="s">
+      <c r="A154" s="1" t="s">
+        <v>1270</v>
+      </c>
+      <c r="M154" t="s">
+        <v>1273</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A155" s="1" t="s">
+        <v>1271</v>
+      </c>
+      <c r="M155" s="2" t="s">
+        <v>1272</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A156" t="s">
         <v>1123</v>
       </c>
-      <c r="M154" t="s">
+      <c r="M156" t="s">
         <v>1127</v>
-      </c>
-    </row>
-    <row r="155" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A155" t="s">
-        <v>1124</v>
-      </c>
-      <c r="M155" t="s">
-        <v>1126</v>
-      </c>
-    </row>
-    <row r="156" spans="1:13" ht="153" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A156" t="s">
-        <v>1125</v>
-      </c>
-      <c r="M156" s="2" t="s">
-        <v>1169</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="M157" t="s">
-        <v>1131</v>
-      </c>
-    </row>
-    <row r="158" spans="1:13" x14ac:dyDescent="0.4">
+        <v>1126</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" ht="150" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
-        <v>1129</v>
-      </c>
-      <c r="M158" t="s">
-        <v>1132</v>
+        <v>1125</v>
+      </c>
+      <c r="M158" s="2" t="s">
+        <v>1274</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
+        <v>1128</v>
+      </c>
+      <c r="M159" t="s">
+        <v>1131</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A160" t="s">
+        <v>1129</v>
+      </c>
+      <c r="M160" t="s">
+        <v>1132</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A161" t="s">
         <v>1130</v>
       </c>
-      <c r="M159" t="s">
+      <c r="M161" t="s">
         <v>1133</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A163" t="s">
+        <v>1285</v>
+      </c>
+      <c r="M163" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A164" s="1" t="s">
+        <v>1284</v>
+      </c>
+      <c r="M164" t="s">
+        <v>1286</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A165" s="1" t="s">
+        <v>1275</v>
+      </c>
+      <c r="M165" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A166" s="1" t="s">
+        <v>1276</v>
+      </c>
+      <c r="M166" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A167" s="1" t="s">
+        <v>1277</v>
+      </c>
+      <c r="M167" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A168" s="1" t="s">
+        <v>1278</v>
+      </c>
+      <c r="M168" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A169" s="1" t="s">
+        <v>1279</v>
+      </c>
+      <c r="M169" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A170" s="1" t="s">
+        <v>1280</v>
+      </c>
+      <c r="M170" t="s">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A171" s="1" t="s">
+        <v>1281</v>
+      </c>
+      <c r="M171" t="s">
+        <v>1289</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A172" s="1" t="s">
+        <v>1282</v>
+      </c>
+      <c r="M172" t="s">
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A173" s="1" t="s">
+        <v>1283</v>
+      </c>
+      <c r="M173" t="s">
+        <v>1290</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A174" s="1" t="s">
+        <v>1294</v>
+      </c>
+      <c r="M174" t="s">
+        <v>1292</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A175" t="s">
+        <v>1295</v>
+      </c>
+      <c r="M175" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A176" s="1" t="s">
+        <v>1310</v>
+      </c>
+      <c r="M176" t="s">
+        <v>1293</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A177" t="s">
+        <v>1311</v>
+      </c>
+      <c r="M177" t="s">
+        <v>1314</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A178" t="s">
+        <v>1312</v>
+      </c>
+      <c r="M178" t="s">
+        <v>1315</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A179" t="s">
+        <v>1313</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A180" t="s">
+        <v>1316</v>
+      </c>
+      <c r="M180" t="s">
+        <v>1317</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A181" t="s">
+        <v>1318</v>
+      </c>
+      <c r="M181" t="s">
+        <v>1319</v>
+      </c>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A183" s="1" t="s">
+        <v>1304</v>
+      </c>
+      <c r="M183" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A184" s="1" t="s">
+        <v>1296</v>
+      </c>
+      <c r="M184" t="s">
+        <v>1305</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A185" s="1" t="s">
+        <v>1297</v>
+      </c>
+      <c r="M185" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A186" s="1" t="s">
+        <v>1298</v>
+      </c>
+      <c r="M186" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A187" s="1" t="s">
+        <v>1299</v>
+      </c>
+      <c r="M187" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A188" s="1" t="s">
+        <v>1300</v>
+      </c>
+      <c r="M188" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A189" s="1" t="s">
+        <v>1301</v>
+      </c>
+      <c r="M189" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A190" s="1" t="s">
+        <v>1302</v>
+      </c>
+      <c r="M190" t="s">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A191" s="1" t="s">
+        <v>1303</v>
+      </c>
+      <c r="M191" t="s">
+        <v>1308</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A192" s="1" t="s">
+        <v>1322</v>
+      </c>
+      <c r="M192" t="s">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A193" t="s">
+        <v>1323</v>
+      </c>
+      <c r="M193" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A194" t="s">
+        <v>1324</v>
+      </c>
+      <c r="M194" t="s">
+        <v>1327</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A195" t="s">
+        <v>1325</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A196" t="s">
+        <v>1320</v>
+      </c>
+      <c r="M196" t="s">
+        <v>1321</v>
       </c>
     </row>
   </sheetData>
@@ -11676,10 +12921,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131ED9DB-7094-4FCA-8832-3F1005AB8270}">
-  <dimension ref="A1:Q212"/>
+  <dimension ref="A1:Q255"/>
   <sheetViews>
-    <sheetView topLeftCell="A196" workbookViewId="0">
-      <selection activeCell="M211" sqref="M211"/>
+    <sheetView topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="E224" sqref="E224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -13338,6 +14583,328 @@
         <v>1114</v>
       </c>
     </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A214" t="s">
+        <v>1227</v>
+      </c>
+      <c r="M214" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A215" s="1" t="s">
+        <v>1226</v>
+      </c>
+      <c r="M215" t="s">
+        <v>1228</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A216" s="1" t="s">
+        <v>1209</v>
+      </c>
+      <c r="M216" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A217" s="1" t="s">
+        <v>1210</v>
+      </c>
+      <c r="M217" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A218" s="1" t="s">
+        <v>1211</v>
+      </c>
+      <c r="M218" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A219" s="1" t="s">
+        <v>1212</v>
+      </c>
+      <c r="M219" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A220" s="1" t="s">
+        <v>1213</v>
+      </c>
+      <c r="M220" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A221" s="1" t="s">
+        <v>1214</v>
+      </c>
+      <c r="M221" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A222" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="M222" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A223" s="1" t="s">
+        <v>1216</v>
+      </c>
+      <c r="M223" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A224" s="1" t="s">
+        <v>1217</v>
+      </c>
+      <c r="M224" t="s">
+        <v>1232</v>
+      </c>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A225" s="1" t="s">
+        <v>1218</v>
+      </c>
+      <c r="M225" t="s">
+        <v>1257</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A226" s="1" t="s">
+        <v>1219</v>
+      </c>
+      <c r="M226" t="s">
+        <v>1230</v>
+      </c>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A227" s="1" t="s">
+        <v>1220</v>
+      </c>
+      <c r="M227" t="s">
+        <v>1229</v>
+      </c>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A228" s="1" t="s">
+        <v>1221</v>
+      </c>
+      <c r="M228" t="s">
+        <v>1231</v>
+      </c>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A229" s="1" t="s">
+        <v>1222</v>
+      </c>
+      <c r="M229" t="s">
+        <v>1256</v>
+      </c>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A230" s="1" t="s">
+        <v>1223</v>
+      </c>
+      <c r="M230" t="s">
+        <v>1255</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A231" s="1" t="s">
+        <v>1224</v>
+      </c>
+      <c r="M231" t="s">
+        <v>1233</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A232" s="1" t="s">
+        <v>1225</v>
+      </c>
+      <c r="M232" t="s">
+        <v>1234</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A233" s="1" t="s">
+        <v>1236</v>
+      </c>
+      <c r="M233" t="s">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A234" t="s">
+        <v>1237</v>
+      </c>
+      <c r="M234" t="s">
+        <v>1269</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A235" t="s">
+        <v>1238</v>
+      </c>
+      <c r="M235" t="s">
+        <v>1258</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A236" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A238" t="s">
+        <v>1253</v>
+      </c>
+      <c r="M238" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A239" s="1" t="s">
+        <v>1252</v>
+      </c>
+      <c r="M239" t="s">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A240" s="1" t="s">
+        <v>1240</v>
+      </c>
+      <c r="M240" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A241" s="1" t="s">
+        <v>1241</v>
+      </c>
+      <c r="M241" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A242" s="1" t="s">
+        <v>1242</v>
+      </c>
+      <c r="M242" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A243" s="1" t="s">
+        <v>1243</v>
+      </c>
+      <c r="M243" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A244" s="1" t="s">
+        <v>1244</v>
+      </c>
+      <c r="M244" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A245" s="1" t="s">
+        <v>1245</v>
+      </c>
+      <c r="M245" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A246" s="1" t="s">
+        <v>1246</v>
+      </c>
+      <c r="M246" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A247" s="1" t="s">
+        <v>1247</v>
+      </c>
+      <c r="M247" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A248" s="1" t="s">
+        <v>1248</v>
+      </c>
+      <c r="M248" t="s">
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A249" s="1" t="s">
+        <v>1249</v>
+      </c>
+      <c r="M249" t="s">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A250" s="1" t="s">
+        <v>1250</v>
+      </c>
+      <c r="M250" t="s">
+        <v>1261</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A251" s="1" t="s">
+        <v>1251</v>
+      </c>
+      <c r="M251" t="s">
+        <v>1262</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A252" t="s">
+        <v>1263</v>
+      </c>
+      <c r="M252" t="s">
+        <v>1265</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A253" t="s">
+        <v>1264</v>
+      </c>
+      <c r="M253" t="s">
+        <v>1266</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A254" t="s">
+        <v>1239</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A255" t="s">
+        <v>1267</v>
+      </c>
+      <c r="M255" t="s">
+        <v>1268</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13347,10 +14914,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{445F46B3-1A86-46EF-9440-E5378C8C2CDD}">
-  <dimension ref="A1:Q102"/>
+  <dimension ref="A1:Q122"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+    <sheetView topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="M121" sqref="M121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -14123,66 +15690,218 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A95" s="1" t="s">
-        <v>878</v>
+        <v>1169</v>
       </c>
       <c r="M95" s="1" t="s">
-        <v>895</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A96" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="M96" s="1" t="s">
-        <v>885</v>
+        <v>895</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A97" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="M97" s="1" t="s">
-        <v>896</v>
+        <v>885</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A98" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="M98" s="1" t="s">
+        <v>896</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A99" s="1" t="s">
         <v>889</v>
       </c>
-      <c r="M98" s="1" t="s">
+      <c r="M99" s="1" t="s">
         <v>886</v>
-      </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A99" t="s">
-        <v>890</v>
-      </c>
-      <c r="M99" s="1" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
+        <v>890</v>
+      </c>
+      <c r="M100" s="1" t="s">
+        <v>894</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A101" t="s">
         <v>891</v>
       </c>
-      <c r="M100" s="1" t="s">
+      <c r="M101" s="1" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="266.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
+    <row r="102" spans="1:13" ht="262.5" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
         <v>892</v>
       </c>
-      <c r="M101" s="2" t="s">
+      <c r="M102" s="2" t="s">
         <v>1156</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A102" s="1" t="s">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A103" s="1" t="s">
         <v>887</v>
       </c>
-      <c r="M102" s="1" t="s">
+      <c r="M103" s="1" t="s">
         <v>888</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="M104" s="1"/>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A105" t="s">
+        <v>1183</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A106" s="1" t="s">
+        <v>1182</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>1184</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A107" s="1" t="s">
+        <v>1171</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A108" s="1" t="s">
+        <v>1172</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A109" s="1" t="s">
+        <v>1173</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A110" s="1" t="s">
+        <v>1174</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A111" s="1" t="s">
+        <v>1175</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>1185</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A112" s="1" t="s">
+        <v>1176</v>
+      </c>
+      <c r="M112" s="1" t="s">
+        <v>1186</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A113" s="1" t="s">
+        <v>1177</v>
+      </c>
+      <c r="M113" s="1" t="s">
+        <v>1187</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A114" s="1" t="s">
+        <v>1178</v>
+      </c>
+      <c r="M114" s="1" t="s">
+        <v>1188</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A115" s="1" t="s">
+        <v>1179</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>1191</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A116" s="1" t="s">
+        <v>1180</v>
+      </c>
+      <c r="M116" s="1" t="s">
+        <v>1192</v>
+      </c>
+    </row>
+    <row r="117" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A117" s="1" t="s">
+        <v>1181</v>
+      </c>
+      <c r="M117" s="1" t="s">
+        <v>1189</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A118" s="1" t="s">
+        <v>1193</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>1190</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A119" t="s">
+        <v>1194</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>1197</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A120" t="s">
+        <v>1195</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A121" t="s">
+        <v>1196</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="122" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A122" t="s">
+        <v>1199</v>
       </c>
     </row>
   </sheetData>
@@ -14194,15 +15913,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3747E3-550F-4585-A066-931F491B69D2}">
-  <dimension ref="A1:Q82"/>
+  <dimension ref="A1:Q86"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="38.375" customWidth="1"/>
+    <col min="1" max="1" width="50.375" customWidth="1"/>
     <col min="13" max="13" width="56.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14673,218 +16392,250 @@
       </c>
     </row>
     <row r="55" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A55" t="s">
+      <c r="A55" s="1" t="s">
+        <v>1201</v>
+      </c>
+      <c r="M55" t="s">
+        <v>1205</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A56" s="1" t="s">
+        <v>1202</v>
+      </c>
+      <c r="M56" t="s">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A57" s="1" t="s">
+        <v>1203</v>
+      </c>
+      <c r="M57" t="s">
+        <v>1207</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A58" s="1" t="s">
+        <v>1204</v>
+      </c>
+      <c r="M58" t="s">
+        <v>1208</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A59" t="s">
         <v>210</v>
       </c>
-      <c r="M55" t="s">
+      <c r="M59" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A56" t="s">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A60" t="s">
         <v>211</v>
       </c>
-      <c r="M56" t="s">
+      <c r="M60" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="279" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A57" t="s">
+    <row r="61" spans="1:13" ht="282.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A61" t="s">
         <v>508</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="M61" s="2" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="247.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A58" t="s">
+    <row r="62" spans="1:13" ht="243.75" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>510</v>
       </c>
-      <c r="M58" s="2" t="s">
+      <c r="M62" s="2" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="150" x14ac:dyDescent="0.4">
-      <c r="A59" t="s">
+    <row r="63" spans="1:13" ht="150" x14ac:dyDescent="0.4">
+      <c r="A63" t="s">
         <v>509</v>
       </c>
-      <c r="M59" s="2" t="s">
+      <c r="M63" s="2" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A60" t="s">
+    <row r="64" spans="1:13" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A64" t="s">
         <v>511</v>
       </c>
-      <c r="M60" s="2" t="s">
+      <c r="M64" s="2" t="s">
         <v>610</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A61" t="s">
-        <v>463</v>
-      </c>
-      <c r="M61" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A62" t="s">
-        <v>517</v>
-      </c>
-      <c r="M62" s="2" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A63" t="s">
-        <v>343</v>
-      </c>
-      <c r="M63" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
-        <v>441</v>
+        <v>463</v>
       </c>
       <c r="M65" t="s">
-        <v>442</v>
+        <v>464</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
-        <v>443</v>
-      </c>
-      <c r="M66" t="s">
-        <v>446</v>
+        <v>517</v>
+      </c>
+      <c r="M66" s="2" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
-        <v>444</v>
+        <v>343</v>
       </c>
       <c r="M67" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A68" t="s">
-        <v>447</v>
-      </c>
-      <c r="M68" t="s">
-        <v>442</v>
+        <v>344</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="M69" t="s">
-        <v>133</v>
+        <v>442</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="M70" t="s">
-        <v>171</v>
+        <v>446</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="M71" t="s">
-        <v>172</v>
+        <v>445</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="M72" t="s">
-        <v>404</v>
+        <v>442</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="M73" t="s">
-        <v>405</v>
+        <v>133</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="M74" t="s">
-        <v>104</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="M75" t="s">
-        <v>116</v>
+        <v>172</v>
       </c>
     </row>
     <row r="76" spans="1:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="M76" t="s">
-        <v>115</v>
+        <v>404</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="M77" t="s">
-        <v>117</v>
+        <v>405</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="M78" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="M79" t="s">
-        <v>460</v>
+        <v>116</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
+        <v>455</v>
+      </c>
+      <c r="M80" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A81" t="s">
+        <v>456</v>
+      </c>
+      <c r="M81" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
+        <v>457</v>
+      </c>
+      <c r="M82" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A83" t="s">
+        <v>458</v>
+      </c>
+      <c r="M83" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
         <v>459</v>
       </c>
-      <c r="M80" t="s">
+      <c r="M84" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
+    <row r="85" spans="1:13" ht="174" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A85" t="s">
         <v>512</v>
       </c>
-      <c r="M81" s="2" t="s">
+      <c r="M85" s="2" t="s">
         <v>704</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="A82" t="s">
+    <row r="86" spans="1:13" ht="171" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A86" t="s">
         <v>513</v>
       </c>
-      <c r="M82" s="2" t="s">
+      <c r="M86" s="2" t="s">
         <v>705</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change:AssaultMaster reload logic and show reduce killcool time
</commit_message>
<xml_diff>
--- a/ExtremeRolesTransData.xlsx
+++ b/ExtremeRolesTransData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB449E3-4DD8-4CAE-B238-AFD4BE882BDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9771E739-C6E3-4B2B-A9D7-F43AA409E503}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2040" uniqueCount="1700">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2044" uniqueCount="1704">
   <si>
     <t>English</t>
   </si>
@@ -14170,171 +14170,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>会議が発生する毎に貯まる「ストック」で強化されるインポスター
-能力「ストック」：現在のストック本数:{0}/{1}本
-　・「ストック」は通報及び会議ボタンによって一定数貯まる
-　・通報と会議ボタンで貯まる本数は変わる
-　・所持できる「ストック」の本数には上限がある
-　・上限を超えた「ストック」1本に付き「リロード」のクール
-　タイムが減少する
-能力「リロード」：現在のリロードクールタイム:{2}秒
-　・能力使用時「ストック」を全て消費することで現在のキル
-　クールを大幅に減少させる
-　・能力を使用すると減少していた「リロード」のクールタイム
-　はもとに戻る
-能力「コッキング」：
-　・貯まっている「ストック」を1本使用する事でキルクールを
-　一定値減少させる</t>
-    <rPh sb="0" eb="2">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ハッセイ</t>
-    </rPh>
-    <rPh sb="7" eb="8">
-      <t>ゴト</t>
-    </rPh>
-    <rPh sb="9" eb="10">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>キョウカ</t>
-    </rPh>
-    <rPh sb="31" eb="33">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="40" eb="42">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ホンスウ</t>
-    </rPh>
-    <rPh sb="57" eb="58">
-      <t>ホン</t>
-    </rPh>
-    <rPh sb="68" eb="70">
-      <t>ツウホウ</t>
-    </rPh>
-    <rPh sb="70" eb="71">
-      <t>オヨ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="81" eb="84">
-      <t>イッテイスウ</t>
-    </rPh>
-    <rPh sb="84" eb="85">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>ツウホウ</t>
-    </rPh>
-    <rPh sb="93" eb="95">
-      <t>カイギ</t>
-    </rPh>
-    <rPh sb="99" eb="100">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="102" eb="104">
-      <t>ホンスウ</t>
-    </rPh>
-    <rPh sb="105" eb="106">
-      <t>カ</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>ショジ</t>
-    </rPh>
-    <rPh sb="123" eb="125">
-      <t>ホンスウ</t>
-    </rPh>
-    <rPh sb="127" eb="129">
-      <t>ジョウゲン</t>
-    </rPh>
-    <rPh sb="135" eb="137">
-      <t>ジョウゲン</t>
-    </rPh>
-    <rPh sb="138" eb="139">
-      <t>コ</t>
-    </rPh>
-    <rPh sb="148" eb="149">
-      <t>ポン</t>
-    </rPh>
-    <rPh sb="150" eb="151">
-      <t>ツ</t>
-    </rPh>
-    <rPh sb="168" eb="170">
-      <t>ゲンショウ</t>
-    </rPh>
-    <rPh sb="173" eb="175">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="182" eb="184">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="199" eb="200">
-      <t>ビョウ</t>
-    </rPh>
-    <rPh sb="203" eb="205">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="205" eb="207">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="207" eb="208">
-      <t>ジ</t>
-    </rPh>
-    <rPh sb="215" eb="216">
-      <t>スベ</t>
-    </rPh>
-    <rPh sb="217" eb="219">
-      <t>ショウヒ</t>
-    </rPh>
-    <rPh sb="224" eb="226">
-      <t>ゲンザイ</t>
-    </rPh>
-    <rPh sb="235" eb="237">
-      <t>オオハバ</t>
-    </rPh>
-    <rPh sb="238" eb="240">
-      <t>ゲンショウ</t>
-    </rPh>
-    <rPh sb="246" eb="248">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="249" eb="251">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="254" eb="256">
-      <t>ゲンショウ</t>
-    </rPh>
-    <rPh sb="279" eb="280">
-      <t>モド</t>
-    </rPh>
-    <rPh sb="282" eb="284">
-      <t>ノウリョク</t>
-    </rPh>
-    <rPh sb="295" eb="296">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="309" eb="310">
-      <t>ポン</t>
-    </rPh>
-    <rPh sb="310" eb="312">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="314" eb="315">
-      <t>コト</t>
-    </rPh>
-    <rPh sb="324" eb="327">
-      <t>イッテイチ</t>
-    </rPh>
-    <rPh sb="327" eb="329">
-      <t>ゲンショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>銃と弾の扱いはお手の物！！</t>
     <rPh sb="0" eb="1">
       <t>ジュウ</t>
@@ -14498,6 +14333,206 @@
     </rPh>
     <rPh sb="301" eb="305">
       <t>ジッコウカノウ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>noStockNow</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>reduceKillCool</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ストック無し</t>
+    <rPh sb="4" eb="5">
+      <t>ナ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>キルクール\n最大{0}秒減少可</t>
+    <rPh sb="7" eb="9">
+      <t>サイダイ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>ビョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ゲンショウ</t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t>カ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>会議が発生する毎に貯まる「ストック」で強化されるインポスター
+パッシブ能力「ストック」：現在のストック本数:{0}/{1}本
+　・「ストック」は通報及び会議ボタンによって一定数貯まる
+　・通報と会議ボタンで貯まる本数は変わる
+　・所持できる「ストック」の本数には上限がある
+　・上限を超えた「ストック」1本に付き「リロード」のクール
+　タイムが減少する
+ボタン能力「リロード」：現在のリロードクールタイム:{2}秒
+　・能力使用時「ストック」を使えるだけ消費して現在のキル
+　クールを大幅に減らす
+　・能力を使用すると減少していた「リロード」のクールタイム
+　はもとに戻る
+パッシブ能力「コッキング」：
+　・キル時に自動発動する
+　・貯まっている「ストック」を1本使用する事でキルクールを
+　一定値減少させる</t>
+    <rPh sb="0" eb="2">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ハッセイ</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>ゴト</t>
+    </rPh>
+    <rPh sb="9" eb="10">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="19" eb="21">
+      <t>キョウカ</t>
+    </rPh>
+    <rPh sb="35" eb="37">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="44" eb="46">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="51" eb="53">
+      <t>ホンスウ</t>
+    </rPh>
+    <rPh sb="61" eb="62">
+      <t>ホン</t>
+    </rPh>
+    <rPh sb="72" eb="74">
+      <t>ツウホウ</t>
+    </rPh>
+    <rPh sb="74" eb="75">
+      <t>オヨ</t>
+    </rPh>
+    <rPh sb="76" eb="78">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="85" eb="88">
+      <t>イッテイスウ</t>
+    </rPh>
+    <rPh sb="88" eb="89">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="94" eb="96">
+      <t>ツウホウ</t>
+    </rPh>
+    <rPh sb="97" eb="99">
+      <t>カイギ</t>
+    </rPh>
+    <rPh sb="103" eb="104">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="106" eb="108">
+      <t>ホンスウ</t>
+    </rPh>
+    <rPh sb="109" eb="110">
+      <t>カ</t>
+    </rPh>
+    <rPh sb="115" eb="117">
+      <t>ショジ</t>
+    </rPh>
+    <rPh sb="127" eb="129">
+      <t>ホンスウ</t>
+    </rPh>
+    <rPh sb="131" eb="133">
+      <t>ジョウゲン</t>
+    </rPh>
+    <rPh sb="139" eb="141">
+      <t>ジョウゲン</t>
+    </rPh>
+    <rPh sb="142" eb="143">
+      <t>コ</t>
+    </rPh>
+    <rPh sb="152" eb="153">
+      <t>ポン</t>
+    </rPh>
+    <rPh sb="154" eb="155">
+      <t>ツ</t>
+    </rPh>
+    <rPh sb="172" eb="174">
+      <t>ゲンショウ</t>
+    </rPh>
+    <rPh sb="180" eb="182">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="189" eb="191">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="206" eb="207">
+      <t>ビョウ</t>
+    </rPh>
+    <rPh sb="210" eb="212">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="212" eb="214">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="214" eb="215">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="222" eb="224">
+      <t>ショウヒ</t>
+    </rPh>
+    <rPh sb="226" eb="228">
+      <t>ゲンザイ</t>
+    </rPh>
+    <rPh sb="237" eb="239">
+      <t>オオハバ</t>
+    </rPh>
+    <rPh sb="240" eb="241">
+      <t>ヘ</t>
+    </rPh>
+    <rPh sb="246" eb="248">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="249" eb="251">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="254" eb="256">
+      <t>ゲンショウ</t>
+    </rPh>
+    <rPh sb="279" eb="280">
+      <t>モド</t>
+    </rPh>
+    <rPh sb="286" eb="288">
+      <t>ノウリョク</t>
+    </rPh>
+    <rPh sb="301" eb="302">
+      <t>ジ</t>
+    </rPh>
+    <rPh sb="303" eb="307">
+      <t>ジドウハツドウ</t>
+    </rPh>
+    <rPh sb="312" eb="313">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="326" eb="327">
+      <t>ポン</t>
+    </rPh>
+    <rPh sb="327" eb="329">
+      <t>シヨウ</t>
+    </rPh>
+    <rPh sb="331" eb="332">
+      <t>コト</t>
+    </rPh>
+    <rPh sb="341" eb="344">
+      <t>イッテイチ</t>
+    </rPh>
+    <rPh sb="344" eb="346">
+      <t>ゲンショウ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -16098,7 +16133,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A5C264A-D4F8-4177-9D21-7A3435066086}">
   <dimension ref="A1:Q241"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B226" workbookViewId="0">
+    <sheetView topLeftCell="B235" workbookViewId="0">
       <selection activeCell="L238" sqref="L238"/>
     </sheetView>
   </sheetViews>
@@ -16796,7 +16831,7 @@
         <v>1596</v>
       </c>
       <c r="M87" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.4">
@@ -17924,7 +17959,7 @@
         <v>1622</v>
       </c>
       <c r="M238" s="2" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="239" spans="1:13" x14ac:dyDescent="0.4">
@@ -17960,9 +17995,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{131ED9DB-7094-4FCA-8832-3F1005AB8270}">
-  <dimension ref="A1:Q296"/>
+  <dimension ref="A1:Q298"/>
   <sheetViews>
-    <sheetView topLeftCell="A290" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B293" workbookViewId="0">
       <selection activeCell="M295" sqref="M295"/>
     </sheetView>
   </sheetViews>
@@ -20235,7 +20270,7 @@
         <v>1690</v>
       </c>
       <c r="M293" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="294" spans="1:13" x14ac:dyDescent="0.4">
@@ -20246,12 +20281,12 @@
         <v>1695</v>
       </c>
     </row>
-    <row r="295" spans="1:13" ht="301.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="295" spans="1:13" ht="321.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A295" t="s">
         <v>1692</v>
       </c>
       <c r="M295" s="2" t="s">
-        <v>1696</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="296" spans="1:13" x14ac:dyDescent="0.4">
@@ -20260,6 +20295,22 @@
       </c>
       <c r="M296" t="s">
         <v>1694</v>
+      </c>
+    </row>
+    <row r="297" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A297" t="s">
+        <v>1699</v>
+      </c>
+      <c r="M297" t="s">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="298" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A298" t="s">
+        <v>1700</v>
+      </c>
+      <c r="M298" t="s">
+        <v>1702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix: text-99 " ," → ", "
</commit_message>
<xml_diff>
--- a/ExtremeRolesTransData.xlsx
+++ b/ExtremeRolesTransData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GIT\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD11DFF5-6B12-4B4D-843D-4A2D8EDFF4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F866DDFF-4A64-479B-99D3-C4E8F496632F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25890" yWindow="-5655" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5799" uniqueCount="4275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5799" uniqueCount="4276">
   <si>
     <t>English</t>
   </si>
@@ -19423,10 +19423,6 @@
     <phoneticPr fontId="6" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> , </t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
     <t>"PORTAL" : Player detection range</t>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
@@ -19945,6 +19941,14 @@
   <si>
     <t>"CAPTURE" : Ability charges</t>
     <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>Disconnected</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">,  </t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -20438,8 +20442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q289"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M104" sqref="M104"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -21621,7 +21625,7 @@
         <v>274</v>
       </c>
       <c r="B92" s="18" t="s">
-        <v>4265</v>
+        <v>4264</v>
       </c>
       <c r="M92" t="s">
         <v>275</v>
@@ -21635,7 +21639,7 @@
         <v>277</v>
       </c>
       <c r="B93" s="18" t="s">
-        <v>4264</v>
+        <v>4263</v>
       </c>
       <c r="M93" t="s">
         <v>278</v>
@@ -21663,7 +21667,7 @@
         <v>283</v>
       </c>
       <c r="B95" s="18" t="s">
-        <v>4263</v>
+        <v>4262</v>
       </c>
       <c r="O95" s="10" t="s">
         <v>284</v>
@@ -21713,7 +21717,7 @@
         <v>292</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>4147</v>
+        <v>4275</v>
       </c>
       <c r="M100" t="s">
         <v>293</v>
@@ -22371,7 +22375,7 @@
         <v>434</v>
       </c>
       <c r="B162" s="15" t="s">
-        <v>4262</v>
+        <v>4261</v>
       </c>
       <c r="M162" t="s">
         <v>435</v>
@@ -22497,7 +22501,7 @@
         <v>459</v>
       </c>
       <c r="B172" s="22" t="s">
-        <v>459</v>
+        <v>4274</v>
       </c>
       <c r="M172" t="s">
         <v>460</v>
@@ -24212,8 +24216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" workbookViewId="0">
-      <selection activeCell="J290" sqref="J290"/>
+    <sheetView topLeftCell="A339" workbookViewId="0">
+      <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -27652,7 +27656,7 @@
         <v>1261</v>
       </c>
       <c r="B260" s="15" t="s">
-        <v>4260</v>
+        <v>4259</v>
       </c>
       <c r="M260" t="s">
         <v>1262</v>
@@ -27806,7 +27810,7 @@
         <v>1285</v>
       </c>
       <c r="B273" s="12" t="s">
-        <v>4273</v>
+        <v>4272</v>
       </c>
       <c r="M273" t="s">
         <v>1286</v>
@@ -27820,7 +27824,7 @@
         <v>1288</v>
       </c>
       <c r="B274" s="12" t="s">
-        <v>4272</v>
+        <v>4271</v>
       </c>
       <c r="M274" t="s">
         <v>1289</v>
@@ -27982,7 +27986,7 @@
         <v>1315</v>
       </c>
       <c r="B287" s="12" t="s">
-        <v>4270</v>
+        <v>4269</v>
       </c>
       <c r="M287" t="s">
         <v>1316</v>
@@ -27996,7 +28000,7 @@
         <v>1318</v>
       </c>
       <c r="B288" s="12" t="s">
-        <v>4271</v>
+        <v>4270</v>
       </c>
       <c r="M288" t="s">
         <v>1319</v>
@@ -28049,7 +28053,7 @@
         <v>1330</v>
       </c>
       <c r="B292" s="12" t="s">
-        <v>4274</v>
+        <v>4273</v>
       </c>
       <c r="M292" t="s">
         <v>1331</v>
@@ -28306,7 +28310,7 @@
         <v>1378</v>
       </c>
       <c r="B312" s="12" t="s">
-        <v>4266</v>
+        <v>4265</v>
       </c>
       <c r="M312" t="s">
         <v>1379</v>
@@ -28331,7 +28335,7 @@
         <v>1384</v>
       </c>
       <c r="B314" s="12" t="s">
-        <v>4267</v>
+        <v>4266</v>
       </c>
       <c r="M314" t="s">
         <v>1385</v>
@@ -28345,7 +28349,7 @@
         <v>1387</v>
       </c>
       <c r="B315" s="12" t="s">
-        <v>4268</v>
+        <v>4267</v>
       </c>
       <c r="M315" t="s">
         <v>1388</v>
@@ -28359,7 +28363,7 @@
         <v>1390</v>
       </c>
       <c r="B316" s="12" t="s">
-        <v>4269</v>
+        <v>4268</v>
       </c>
       <c r="M316" t="s">
         <v>1391</v>
@@ -28668,7 +28672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q425"/>
   <sheetViews>
-    <sheetView topLeftCell="A258" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A398" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J255" sqref="J255"/>
     </sheetView>
   </sheetViews>
@@ -28751,7 +28755,7 @@
         <v>1456</v>
       </c>
       <c r="B3" s="50" t="s">
-        <v>4165</v>
+        <v>4164</v>
       </c>
       <c r="M3" s="2" t="s">
         <v>1457</v>
@@ -29169,7 +29173,7 @@
         <v>1514</v>
       </c>
       <c r="B35" s="49" t="s">
-        <v>4166</v>
+        <v>4165</v>
       </c>
       <c r="M35" t="s">
         <v>1515</v>
@@ -29183,7 +29187,7 @@
         <v>1517</v>
       </c>
       <c r="B36" s="49" t="s">
-        <v>4167</v>
+        <v>4166</v>
       </c>
       <c r="M36" t="s">
         <v>1518</v>
@@ -29655,7 +29659,7 @@
         <v>1583</v>
       </c>
       <c r="B72" s="49" t="s">
-        <v>4168</v>
+        <v>4167</v>
       </c>
       <c r="M72" t="s">
         <v>1584</v>
@@ -29669,7 +29673,7 @@
         <v>1586</v>
       </c>
       <c r="B73" s="49" t="s">
-        <v>4169</v>
+        <v>4168</v>
       </c>
       <c r="M73" t="s">
         <v>1587</v>
@@ -29683,7 +29687,7 @@
         <v>1589</v>
       </c>
       <c r="B74" s="49" t="s">
-        <v>4170</v>
+        <v>4169</v>
       </c>
       <c r="M74" t="s">
         <v>1590</v>
@@ -29697,7 +29701,7 @@
         <v>1592</v>
       </c>
       <c r="B75" s="49" t="s">
-        <v>4171</v>
+        <v>4170</v>
       </c>
       <c r="M75" t="s">
         <v>1593</v>
@@ -30119,7 +30123,7 @@
         <v>1651</v>
       </c>
       <c r="B108" s="49" t="s">
-        <v>4172</v>
+        <v>4171</v>
       </c>
       <c r="M108" t="s">
         <v>1652</v>
@@ -30133,7 +30137,7 @@
         <v>1653</v>
       </c>
       <c r="B109" s="49" t="s">
-        <v>4173</v>
+        <v>4172</v>
       </c>
       <c r="M109" t="s">
         <v>1654</v>
@@ -30147,7 +30151,7 @@
         <v>1656</v>
       </c>
       <c r="B110" s="49" t="s">
-        <v>4174</v>
+        <v>4173</v>
       </c>
       <c r="M110" t="s">
         <v>1657</v>
@@ -30355,7 +30359,7 @@
         <v>1684</v>
       </c>
       <c r="B126" s="15" t="s">
-        <v>4175</v>
+        <v>4174</v>
       </c>
       <c r="M126" t="s">
         <v>1685</v>
@@ -30580,7 +30584,7 @@
         <v>1711</v>
       </c>
       <c r="B144" s="49" t="s">
-        <v>4181</v>
+        <v>4180</v>
       </c>
       <c r="M144" t="s">
         <v>1712</v>
@@ -30591,7 +30595,7 @@
         <v>1713</v>
       </c>
       <c r="B145" s="49" t="s">
-        <v>4180</v>
+        <v>4179</v>
       </c>
       <c r="M145" t="s">
         <v>1714</v>
@@ -30602,7 +30606,7 @@
         <v>1715</v>
       </c>
       <c r="B146" s="49" t="s">
-        <v>4176</v>
+        <v>4175</v>
       </c>
       <c r="M146" t="s">
         <v>1716</v>
@@ -30616,7 +30620,7 @@
         <v>1717</v>
       </c>
       <c r="B147" s="49" t="s">
-        <v>4177</v>
+        <v>4176</v>
       </c>
       <c r="M147" t="s">
         <v>1718</v>
@@ -30630,7 +30634,7 @@
         <v>1719</v>
       </c>
       <c r="B148" s="49" t="s">
-        <v>4178</v>
+        <v>4177</v>
       </c>
       <c r="M148" t="s">
         <v>1720</v>
@@ -30644,7 +30648,7 @@
         <v>1722</v>
       </c>
       <c r="B149" s="49" t="s">
-        <v>4179</v>
+        <v>4178</v>
       </c>
       <c r="M149" t="s">
         <v>1723</v>
@@ -30866,7 +30870,7 @@
         <v>1753</v>
       </c>
       <c r="B166" s="49" t="s">
-        <v>4182</v>
+        <v>4181</v>
       </c>
       <c r="M166" t="s">
         <v>1754</v>
@@ -30880,7 +30884,7 @@
         <v>1755</v>
       </c>
       <c r="B167" s="12" t="s">
-        <v>4183</v>
+        <v>4182</v>
       </c>
       <c r="M167" t="s">
         <v>1756</v>
@@ -30894,7 +30898,7 @@
         <v>1757</v>
       </c>
       <c r="B168" s="49" t="s">
-        <v>4184</v>
+        <v>4183</v>
       </c>
       <c r="M168" t="s">
         <v>1758</v>
@@ -30908,7 +30912,7 @@
         <v>1759</v>
       </c>
       <c r="B169" s="49" t="s">
-        <v>4185</v>
+        <v>4184</v>
       </c>
       <c r="M169" t="s">
         <v>1760</v>
@@ -31130,7 +31134,7 @@
         <v>1789</v>
       </c>
       <c r="B186" s="56" t="s">
-        <v>4186</v>
+        <v>4185</v>
       </c>
       <c r="M186" t="s">
         <v>1790</v>
@@ -31144,7 +31148,7 @@
         <v>1791</v>
       </c>
       <c r="B187" s="56" t="s">
-        <v>4187</v>
+        <v>4186</v>
       </c>
       <c r="M187" t="s">
         <v>1792</v>
@@ -31158,7 +31162,7 @@
         <v>1793</v>
       </c>
       <c r="B188" s="49" t="s">
-        <v>4188</v>
+        <v>4187</v>
       </c>
       <c r="M188" t="s">
         <v>1794</v>
@@ -31172,7 +31176,7 @@
         <v>1796</v>
       </c>
       <c r="B189" s="49" t="s">
-        <v>4189</v>
+        <v>4188</v>
       </c>
       <c r="M189" t="s">
         <v>1797</v>
@@ -31186,7 +31190,7 @@
         <v>1799</v>
       </c>
       <c r="B190" s="56" t="s">
-        <v>4191</v>
+        <v>4190</v>
       </c>
       <c r="M190" t="s">
         <v>1800</v>
@@ -31200,7 +31204,7 @@
         <v>1802</v>
       </c>
       <c r="B191" s="56" t="s">
-        <v>4190</v>
+        <v>4189</v>
       </c>
       <c r="M191" t="s">
         <v>1803</v>
@@ -31214,7 +31218,7 @@
         <v>1805</v>
       </c>
       <c r="B192" s="49" t="s">
-        <v>4192</v>
+        <v>4191</v>
       </c>
       <c r="M192" t="s">
         <v>1806</v>
@@ -31478,7 +31482,7 @@
         <v>1844</v>
       </c>
       <c r="B212" s="56" t="s">
-        <v>4148</v>
+        <v>4147</v>
       </c>
       <c r="M212" t="s">
         <v>1845</v>
@@ -31506,7 +31510,7 @@
         <v>1850</v>
       </c>
       <c r="B214" s="49" t="s">
-        <v>4193</v>
+        <v>4192</v>
       </c>
       <c r="M214" t="s">
         <v>1851</v>
@@ -31995,7 +31999,7 @@
         <v>1925</v>
       </c>
       <c r="B253" s="49" t="s">
-        <v>4261</v>
+        <v>4260</v>
       </c>
       <c r="M253" t="s">
         <v>1926</v>
@@ -32009,7 +32013,7 @@
         <v>1928</v>
       </c>
       <c r="B254" s="56" t="s">
-        <v>4149</v>
+        <v>4148</v>
       </c>
       <c r="M254" t="s">
         <v>1929</v>
@@ -32023,7 +32027,7 @@
         <v>1931</v>
       </c>
       <c r="B255" s="56" t="s">
-        <v>4150</v>
+        <v>4149</v>
       </c>
       <c r="M255" t="s">
         <v>1932</v>
@@ -32231,7 +32235,7 @@
         <v>1959</v>
       </c>
       <c r="B271" s="49" t="s">
-        <v>4151</v>
+        <v>4150</v>
       </c>
       <c r="M271" t="s">
         <v>1960</v>
@@ -32245,7 +32249,7 @@
         <v>1962</v>
       </c>
       <c r="B272" s="49" t="s">
-        <v>4152</v>
+        <v>4151</v>
       </c>
       <c r="M272" t="s">
         <v>1963</v>
@@ -32259,7 +32263,7 @@
         <v>1964</v>
       </c>
       <c r="B273" s="49" t="s">
-        <v>4153</v>
+        <v>4152</v>
       </c>
       <c r="M273" t="s">
         <v>1965</v>
@@ -32273,7 +32277,7 @@
         <v>1967</v>
       </c>
       <c r="B274" s="12" t="s">
-        <v>4154</v>
+        <v>4153</v>
       </c>
       <c r="M274" t="s">
         <v>1968</v>
@@ -32784,7 +32788,7 @@
         <v>2047</v>
       </c>
       <c r="B314" s="49" t="s">
-        <v>4163</v>
+        <v>4162</v>
       </c>
       <c r="M314" t="s">
         <v>2048</v>
@@ -32798,7 +32802,7 @@
         <v>2050</v>
       </c>
       <c r="B315" s="49" t="s">
-        <v>4164</v>
+        <v>4163</v>
       </c>
       <c r="M315" t="s">
         <v>2051</v>
@@ -32812,7 +32816,7 @@
         <v>2053</v>
       </c>
       <c r="B316" s="49" t="s">
-        <v>4160</v>
+        <v>4159</v>
       </c>
       <c r="M316" t="s">
         <v>2054</v>
@@ -32826,7 +32830,7 @@
         <v>2056</v>
       </c>
       <c r="B317" s="49" t="s">
-        <v>4156</v>
+        <v>4155</v>
       </c>
       <c r="M317" t="s">
         <v>2057</v>
@@ -32840,7 +32844,7 @@
         <v>2059</v>
       </c>
       <c r="B318" s="49" t="s">
-        <v>4157</v>
+        <v>4156</v>
       </c>
       <c r="M318" t="s">
         <v>2060</v>
@@ -32854,7 +32858,7 @@
         <v>2062</v>
       </c>
       <c r="B319" s="49" t="s">
-        <v>4158</v>
+        <v>4157</v>
       </c>
       <c r="M319" t="s">
         <v>2063</v>
@@ -32868,7 +32872,7 @@
         <v>2065</v>
       </c>
       <c r="B320" s="49" t="s">
-        <v>4159</v>
+        <v>4158</v>
       </c>
       <c r="M320" t="s">
         <v>2066</v>
@@ -32882,7 +32886,7 @@
         <v>2068</v>
       </c>
       <c r="B321" s="49" t="s">
-        <v>4161</v>
+        <v>4160</v>
       </c>
       <c r="M321" t="s">
         <v>2069</v>
@@ -32896,7 +32900,7 @@
         <v>2071</v>
       </c>
       <c r="B322" s="49" t="s">
-        <v>4155</v>
+        <v>4154</v>
       </c>
       <c r="M322" t="s">
         <v>2072</v>
@@ -32910,7 +32914,7 @@
         <v>2074</v>
       </c>
       <c r="B323" s="49" t="s">
-        <v>4162</v>
+        <v>4161</v>
       </c>
       <c r="M323" t="s">
         <v>2075</v>
@@ -32924,7 +32928,7 @@
         <v>2077</v>
       </c>
       <c r="B324" s="49" t="s">
-        <v>4155</v>
+        <v>4154</v>
       </c>
       <c r="M324" t="s">
         <v>2078</v>
@@ -34169,7 +34173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q262"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A244" workbookViewId="0">
       <selection activeCell="B221" sqref="B221"/>
     </sheetView>
   </sheetViews>
@@ -34378,7 +34382,7 @@
         <v>2312</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>4195</v>
+        <v>4194</v>
       </c>
       <c r="M12" s="1" t="s">
         <v>2313</v>
@@ -34392,7 +34396,7 @@
         <v>2315</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>4196</v>
+        <v>4195</v>
       </c>
       <c r="M13" t="s">
         <v>2316</v>
@@ -34406,7 +34410,7 @@
         <v>2318</v>
       </c>
       <c r="B14" s="56" t="s">
-        <v>4197</v>
+        <v>4196</v>
       </c>
       <c r="M14" t="s">
         <v>2319</v>
@@ -34420,7 +34424,7 @@
         <v>2321</v>
       </c>
       <c r="B15" s="56" t="s">
-        <v>4198</v>
+        <v>4197</v>
       </c>
       <c r="M15" t="s">
         <v>2322</v>
@@ -34434,7 +34438,7 @@
         <v>2324</v>
       </c>
       <c r="B16" s="56" t="s">
-        <v>4199</v>
+        <v>4198</v>
       </c>
       <c r="M16" t="s">
         <v>2325</v>
@@ -34448,7 +34452,7 @@
         <v>2327</v>
       </c>
       <c r="B17" s="56" t="s">
-        <v>4200</v>
+        <v>4199</v>
       </c>
       <c r="M17" t="s">
         <v>2328</v>
@@ -34490,7 +34494,7 @@
         <v>2336</v>
       </c>
       <c r="B20" s="52" t="s">
-        <v>4225</v>
+        <v>4224</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>2337</v>
@@ -34504,7 +34508,7 @@
         <v>2339</v>
       </c>
       <c r="B21" s="51" t="s">
-        <v>4194</v>
+        <v>4193</v>
       </c>
       <c r="M21" t="s">
         <v>2340</v>
@@ -34672,7 +34676,7 @@
         <v>2360</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>4201</v>
+        <v>4200</v>
       </c>
       <c r="M34" s="1" t="s">
         <v>2361</v>
@@ -34686,7 +34690,7 @@
         <v>2363</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>4208</v>
+        <v>4207</v>
       </c>
       <c r="M35" s="1" t="s">
         <v>2364</v>
@@ -34700,7 +34704,7 @@
         <v>2366</v>
       </c>
       <c r="B36" s="51" t="s">
-        <v>4202</v>
+        <v>4201</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>2367</v>
@@ -34714,7 +34718,7 @@
         <v>2369</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>4203</v>
+        <v>4202</v>
       </c>
       <c r="M37" s="1" t="s">
         <v>2370</v>
@@ -34728,7 +34732,7 @@
         <v>2372</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>4204</v>
+        <v>4203</v>
       </c>
       <c r="M38" s="1" t="s">
         <v>2373</v>
@@ -34742,7 +34746,7 @@
         <v>2375</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>4205</v>
+        <v>4204</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>2376</v>
@@ -34756,7 +34760,7 @@
         <v>2378</v>
       </c>
       <c r="B40" s="51" t="s">
-        <v>4206</v>
+        <v>4205</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>2379</v>
@@ -34770,7 +34774,7 @@
         <v>2381</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>4207</v>
+        <v>4206</v>
       </c>
       <c r="M41" s="1" t="s">
         <v>2382</v>
@@ -34784,7 +34788,7 @@
         <v>2384</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>4209</v>
+        <v>4208</v>
       </c>
       <c r="M42" s="1" t="s">
         <v>2385</v>
@@ -34798,7 +34802,7 @@
         <v>2387</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>4210</v>
+        <v>4209</v>
       </c>
       <c r="M43" s="1" t="s">
         <v>2388</v>
@@ -34812,7 +34816,7 @@
         <v>2390</v>
       </c>
       <c r="B44" s="51" t="s">
-        <v>4211</v>
+        <v>4210</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>2391</v>
@@ -34826,7 +34830,7 @@
         <v>2393</v>
       </c>
       <c r="B45" s="51" t="s">
-        <v>4212</v>
+        <v>4211</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>2394</v>
@@ -34840,7 +34844,7 @@
         <v>2396</v>
       </c>
       <c r="B46" s="51" t="s">
-        <v>4213</v>
+        <v>4212</v>
       </c>
       <c r="M46" s="1" t="s">
         <v>2397</v>
@@ -34854,7 +34858,7 @@
         <v>2399</v>
       </c>
       <c r="B47" s="56" t="s">
-        <v>4214</v>
+        <v>4213</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>2400</v>
@@ -34868,7 +34872,7 @@
         <v>2401</v>
       </c>
       <c r="B48" s="56" t="s">
-        <v>4215</v>
+        <v>4214</v>
       </c>
       <c r="M48" s="1" t="s">
         <v>2402</v>
@@ -34882,7 +34886,7 @@
         <v>2403</v>
       </c>
       <c r="B49" s="56" t="s">
-        <v>4216</v>
+        <v>4215</v>
       </c>
       <c r="M49" s="1" t="s">
         <v>2404</v>
@@ -34896,7 +34900,7 @@
         <v>2405</v>
       </c>
       <c r="B50" s="56" t="s">
-        <v>4217</v>
+        <v>4216</v>
       </c>
       <c r="M50" s="1" t="s">
         <v>2406</v>
@@ -34910,7 +34914,7 @@
         <v>2407</v>
       </c>
       <c r="B51" s="56" t="s">
-        <v>4218</v>
+        <v>4217</v>
       </c>
       <c r="M51" s="1" t="s">
         <v>2408</v>
@@ -34924,7 +34928,7 @@
         <v>2409</v>
       </c>
       <c r="B52" s="56" t="s">
-        <v>4219</v>
+        <v>4218</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>2410</v>
@@ -34938,7 +34942,7 @@
         <v>2411</v>
       </c>
       <c r="B53" s="56" t="s">
-        <v>4220</v>
+        <v>4219</v>
       </c>
       <c r="M53" s="1" t="s">
         <v>2412</v>
@@ -34952,7 +34956,7 @@
         <v>2413</v>
       </c>
       <c r="B54" s="51" t="s">
-        <v>4221</v>
+        <v>4220</v>
       </c>
       <c r="M54" t="s">
         <v>2414</v>
@@ -35132,7 +35136,7 @@
         <v>2441</v>
       </c>
       <c r="B68" s="51" t="s">
-        <v>4222</v>
+        <v>4221</v>
       </c>
       <c r="M68" s="1" t="s">
         <v>2442</v>
@@ -35146,7 +35150,7 @@
         <v>2444</v>
       </c>
       <c r="B69" s="51" t="s">
-        <v>4223</v>
+        <v>4222</v>
       </c>
       <c r="M69" s="1" t="s">
         <v>2445</v>
@@ -35160,7 +35164,7 @@
         <v>2447</v>
       </c>
       <c r="B70" s="51" t="s">
-        <v>4224</v>
+        <v>4223</v>
       </c>
       <c r="M70" s="1" t="s">
         <v>2448</v>
@@ -35202,7 +35206,7 @@
         <v>2456</v>
       </c>
       <c r="B73" s="52" t="s">
-        <v>4226</v>
+        <v>4225</v>
       </c>
       <c r="M73" s="2" t="s">
         <v>2457</v>
@@ -35314,7 +35318,7 @@
         <v>2470</v>
       </c>
       <c r="B82" s="51" t="s">
-        <v>4227</v>
+        <v>4226</v>
       </c>
       <c r="M82" s="1" t="s">
         <v>2471</v>
@@ -35538,7 +35542,7 @@
         <v>2507</v>
       </c>
       <c r="B99" s="51" t="s">
-        <v>4229</v>
+        <v>4228</v>
       </c>
       <c r="M99" s="1" t="s">
         <v>2508</v>
@@ -35552,7 +35556,7 @@
         <v>2510</v>
       </c>
       <c r="B100" s="51" t="s">
-        <v>4228</v>
+        <v>4227</v>
       </c>
       <c r="M100" s="1" t="s">
         <v>2511</v>
@@ -35566,7 +35570,7 @@
         <v>2512</v>
       </c>
       <c r="B101" s="51" t="s">
-        <v>4231</v>
+        <v>4230</v>
       </c>
       <c r="M101" s="1" t="s">
         <v>2513</v>
@@ -35580,7 +35584,7 @@
         <v>2515</v>
       </c>
       <c r="B102" s="51" t="s">
-        <v>4230</v>
+        <v>4229</v>
       </c>
       <c r="M102" s="1" t="s">
         <v>2516</v>
@@ -35622,7 +35626,7 @@
         <v>2524</v>
       </c>
       <c r="B105" s="52" t="s">
-        <v>4232</v>
+        <v>4231</v>
       </c>
       <c r="M105" s="2" t="s">
         <v>2525</v>
@@ -36201,7 +36205,7 @@
         <v>2625</v>
       </c>
       <c r="B151" s="15" t="s">
-        <v>4236</v>
+        <v>4235</v>
       </c>
       <c r="M151" s="1" t="s">
         <v>2626</v>
@@ -36215,7 +36219,7 @@
         <v>2628</v>
       </c>
       <c r="B152" s="15" t="s">
-        <v>4233</v>
+        <v>4232</v>
       </c>
       <c r="M152" s="1" t="s">
         <v>2629</v>
@@ -36229,7 +36233,7 @@
         <v>2631</v>
       </c>
       <c r="B153" s="15" t="s">
-        <v>4234</v>
+        <v>4233</v>
       </c>
       <c r="M153" s="1" t="s">
         <v>2632</v>
@@ -36243,7 +36247,7 @@
         <v>2634</v>
       </c>
       <c r="B154" s="15" t="s">
-        <v>4235</v>
+        <v>4234</v>
       </c>
       <c r="M154" s="1" t="s">
         <v>2635</v>
@@ -36408,7 +36412,7 @@
         <v>2662</v>
       </c>
       <c r="B167" s="15" t="s">
-        <v>4238</v>
+        <v>4237</v>
       </c>
       <c r="M167" s="1" t="s">
         <v>2663</v>
@@ -36422,7 +36426,7 @@
         <v>2665</v>
       </c>
       <c r="B168" s="15" t="s">
-        <v>4239</v>
+        <v>4238</v>
       </c>
       <c r="M168" s="1" t="s">
         <v>2666</v>
@@ -36436,7 +36440,7 @@
         <v>2668</v>
       </c>
       <c r="B169" s="15" t="s">
-        <v>4240</v>
+        <v>4239</v>
       </c>
       <c r="M169" s="1" t="s">
         <v>2669</v>
@@ -36450,7 +36454,7 @@
         <v>2671</v>
       </c>
       <c r="B170" s="15" t="s">
-        <v>4241</v>
+        <v>4240</v>
       </c>
       <c r="M170" s="1" t="s">
         <v>2672</v>
@@ -36464,7 +36468,7 @@
         <v>2674</v>
       </c>
       <c r="B171" s="15" t="s">
-        <v>4242</v>
+        <v>4241</v>
       </c>
       <c r="M171" s="1" t="s">
         <v>2675</v>
@@ -36517,7 +36521,7 @@
         <v>2686</v>
       </c>
       <c r="B175" s="12" t="s">
-        <v>4237</v>
+        <v>4236</v>
       </c>
       <c r="M175" t="s">
         <v>2687</v>
@@ -36615,7 +36619,7 @@
         <v>2699</v>
       </c>
       <c r="B183" s="15" t="s">
-        <v>4243</v>
+        <v>4242</v>
       </c>
       <c r="M183" s="1" t="s">
         <v>2589</v>
@@ -36629,7 +36633,7 @@
         <v>2701</v>
       </c>
       <c r="B184" s="15" t="s">
-        <v>4244</v>
+        <v>4243</v>
       </c>
       <c r="M184" s="1" t="s">
         <v>2702</v>
@@ -36643,7 +36647,7 @@
         <v>2704</v>
       </c>
       <c r="B185" s="15" t="s">
-        <v>4245</v>
+        <v>4244</v>
       </c>
       <c r="M185" s="1" t="s">
         <v>2705</v>
@@ -36657,7 +36661,7 @@
         <v>2707</v>
       </c>
       <c r="B186" s="15" t="s">
-        <v>4246</v>
+        <v>4245</v>
       </c>
       <c r="M186" s="1" t="s">
         <v>2708</v>
@@ -36685,7 +36689,7 @@
         <v>2713</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>4247</v>
+        <v>4246</v>
       </c>
       <c r="M188" s="1" t="s">
         <v>2714</v>
@@ -36699,7 +36703,7 @@
         <v>2716</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>4248</v>
+        <v>4247</v>
       </c>
       <c r="M189" s="1" t="s">
         <v>2717</v>
@@ -36713,7 +36717,7 @@
         <v>2719</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>4249</v>
+        <v>4248</v>
       </c>
       <c r="M190" s="1" t="s">
         <v>2720</v>
@@ -36727,7 +36731,7 @@
         <v>2722</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>4250</v>
+        <v>4249</v>
       </c>
       <c r="M191" s="1" t="s">
         <v>2723</v>
@@ -36741,7 +36745,7 @@
         <v>2725</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>4251</v>
+        <v>4250</v>
       </c>
       <c r="M192" s="1" t="s">
         <v>2726</v>
@@ -37002,7 +37006,7 @@
         <v>2768</v>
       </c>
       <c r="B212" s="12" t="s">
-        <v>4252</v>
+        <v>4251</v>
       </c>
       <c r="M212" s="1" t="s">
         <v>2769</v>
@@ -37016,7 +37020,7 @@
         <v>2771</v>
       </c>
       <c r="B213" s="12" t="s">
-        <v>4253</v>
+        <v>4252</v>
       </c>
       <c r="M213" s="1" t="s">
         <v>2772</v>
@@ -37030,7 +37034,7 @@
         <v>2774</v>
       </c>
       <c r="B214" s="12" t="s">
-        <v>4254</v>
+        <v>4253</v>
       </c>
       <c r="M214" s="1" t="s">
         <v>2775</v>
@@ -37044,7 +37048,7 @@
         <v>2777</v>
       </c>
       <c r="B215" s="12" t="s">
-        <v>4257</v>
+        <v>4256</v>
       </c>
       <c r="M215" s="1" t="s">
         <v>2778</v>
@@ -37058,7 +37062,7 @@
         <v>2780</v>
       </c>
       <c r="B216" s="12" t="s">
-        <v>4256</v>
+        <v>4255</v>
       </c>
       <c r="M216" s="1" t="s">
         <v>2781</v>
@@ -37072,7 +37076,7 @@
         <v>2783</v>
       </c>
       <c r="B217" s="12" t="s">
-        <v>4255</v>
+        <v>4254</v>
       </c>
       <c r="M217" s="1" t="s">
         <v>2784</v>
@@ -37086,7 +37090,7 @@
         <v>2786</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>4258</v>
+        <v>4257</v>
       </c>
       <c r="M218" s="1" t="s">
         <v>2787</v>
@@ -37637,7 +37641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
@@ -38779,7 +38783,7 @@
         <v>3130</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>4259</v>
+        <v>4258</v>
       </c>
       <c r="M90" s="2" t="s">
         <v>3131</v>

</xml_diff>

<commit_message>
upd: Airship admin settings
</commit_message>
<xml_diff>
--- a/ExtremeRolesTransData.xlsx
+++ b/ExtremeRolesTransData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GIT\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65C000C-CEDD-4339-929F-AC5341A2468C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4D97D0-6465-4D75-A134-9CF1A41D4376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2970" yWindow="4110" windowWidth="25035" windowHeight="12285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2970" yWindow="3195" windowWidth="25035" windowHeight="12285" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6270" uniqueCount="4696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6275" uniqueCount="4701">
   <si>
     <t>English</t>
   </si>
@@ -22628,13 +22628,33 @@
     <phoneticPr fontId="9" type="noConversion"/>
   </si>
   <si>
+    <t>Airship ADMIN settings</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable Both</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable Cockpit only</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable Archive only</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>"RELOAD" : Ability C.D. reduction per STOCK overfilled</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">An IMPOSTOR ability with the ability to reload Kill Cooldowns by using "STOCKS".
 "STOCKS" remaining: {0} / Max {1}
 "RELOAD" will reduce {2} secs on use
 "STOCKS" : A special system for Assault Masters.
  - Can be charged by meetings
- - Cannot stock more than maximum, but can charged even the stocks are maxed out
- - Stocks charged over maximum limits reduces the Ability cooldown of "RELOAD"
+ - Cannot stock more than maximum, but can charged while the stocks are maxed out
+ - Stocks overfilled(charged over maximum limits) reduce the Ability cooldown of "RELOAD"
 "RELOAD" : Reduces the Kill Cooldown by consuming STOCKS on ability usage.
  - On use, resets its ability Cooldown to the initial state.
 "COCKING" : A passive ability automatically activating on Kills
@@ -22832,9 +22852,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="4" applyFill="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -23118,8 +23136,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q295"/>
   <sheetViews>
-    <sheetView topLeftCell="A280" workbookViewId="0">
-      <selection activeCell="B291" sqref="B291"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66:E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -23936,6 +23954,9 @@
       <c r="A61" s="1" t="s">
         <v>4456</v>
       </c>
+      <c r="B61" s="24" t="s">
+        <v>4695</v>
+      </c>
       <c r="M61" s="12" t="s">
         <v>4457</v>
       </c>
@@ -23944,6 +23965,9 @@
       <c r="A62" s="19" t="s">
         <v>4462</v>
       </c>
+      <c r="B62" s="24" t="s">
+        <v>4696</v>
+      </c>
       <c r="M62" s="12" t="s">
         <v>4458</v>
       </c>
@@ -23952,6 +23976,9 @@
       <c r="A63" s="19" t="s">
         <v>4463</v>
       </c>
+      <c r="B63" s="24" t="s">
+        <v>4697</v>
+      </c>
       <c r="M63" s="12" t="s">
         <v>4459</v>
       </c>
@@ -23959,6 +23986,9 @@
     <row r="64" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A64" s="19" t="s">
         <v>4464</v>
+      </c>
+      <c r="B64" s="24" t="s">
+        <v>4698</v>
       </c>
       <c r="M64" s="12" t="s">
         <v>4460</v>
@@ -31401,8 +31431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A333" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B299" sqref="B299"/>
+    <sheetView tabSelected="1" topLeftCell="A299" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D299" sqref="D299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -34616,7 +34646,7 @@
       <c r="A240" t="s">
         <v>1890</v>
       </c>
-      <c r="B240" s="24" t="s">
+      <c r="B240" s="23" t="s">
         <v>4692</v>
       </c>
       <c r="M240" s="2" t="s">
@@ -35358,7 +35388,9 @@
       <c r="A296" s="1" t="s">
         <v>1997</v>
       </c>
-      <c r="B296" s="15"/>
+      <c r="B296" s="22" t="s">
+        <v>4699</v>
+      </c>
       <c r="M296" t="s">
         <v>1998</v>
       </c>
@@ -35394,12 +35426,12 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="299" spans="1:15" ht="375" x14ac:dyDescent="0.4">
+    <row r="299" spans="1:15" ht="393.75" x14ac:dyDescent="0.4">
       <c r="A299" t="s">
         <v>2006</v>
       </c>
       <c r="B299" s="23" t="s">
-        <v>4695</v>
+        <v>4700</v>
       </c>
       <c r="M299" s="2" t="s">
         <v>2007</v>

</xml_diff>

<commit_message>
feat:trans and update custom server check
</commit_message>
<xml_diff>
--- a/ExtremeRolesTransData.xlsx
+++ b/ExtremeRolesTransData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\VisualStudioProject\AmongUs\ExtremeRoles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B073C865-7267-4084-B305-A693C26DCFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3B6363-84C3-415F-91DD-DCA70B95A50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Text" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6908" uniqueCount="5056">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6910" uniqueCount="5058">
   <si>
     <t>English</t>
   </si>
@@ -18922,6 +18922,19 @@
     <t>「ジャグリング」の使用回数</t>
     <rPh sb="9" eb="13">
       <t>シヨウカイスウ</t>
+    </rPh>
+    <phoneticPr fontId="10"/>
+  </si>
+  <si>
+    <t>ExROfficialTokyo</t>
+  </si>
+  <si>
+    <t>ExR専用(東京)</t>
+    <rPh sb="3" eb="5">
+      <t>センヨウ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>トウキョウ</t>
     </rPh>
     <phoneticPr fontId="10"/>
   </si>
@@ -19353,10 +19366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q322"/>
+  <dimension ref="A1:Q323"/>
   <sheetViews>
-    <sheetView topLeftCell="C301" workbookViewId="0">
-      <selection activeCell="M293" sqref="M293"/>
+    <sheetView tabSelected="1" topLeftCell="C67" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="18.75"/>
@@ -20345,1093 +20358,1089 @@
         <v>273</v>
       </c>
     </row>
-    <row r="80" spans="1:15">
-      <c r="A80" t="s">
-        <v>274</v>
-      </c>
-      <c r="B80" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="M80" t="s">
-        <v>276</v>
-      </c>
-      <c r="O80" s="17" t="s">
-        <v>277</v>
-      </c>
+    <row r="79" spans="1:15">
+      <c r="A79" t="s">
+        <v>5056</v>
+      </c>
+      <c r="B79" s="3"/>
+      <c r="M79" s="19" t="s">
+        <v>5057</v>
+      </c>
+      <c r="O79" s="17"/>
     </row>
     <row r="81" spans="1:15">
       <c r="A81" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="M81" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="O81" s="17" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="82" spans="1:15">
       <c r="A82" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="M82" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="O82" s="17" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="83" spans="1:15">
       <c r="A83" t="s">
+        <v>282</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="M83" t="s">
+        <v>284</v>
+      </c>
+      <c r="O83" s="17" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15">
+      <c r="A84" t="s">
         <v>286</v>
       </c>
-      <c r="B83" s="7" t="s">
+      <c r="B84" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="M83" t="s">
+      <c r="M84" t="s">
         <v>288</v>
       </c>
-      <c r="O83" s="17" t="s">
+      <c r="O84" s="17" t="s">
         <v>289</v>
-      </c>
-    </row>
-    <row r="85" spans="1:15">
-      <c r="A85" t="s">
-        <v>290</v>
-      </c>
-      <c r="B85" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="M85" t="s">
-        <v>292</v>
-      </c>
-      <c r="O85" s="17" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="86" spans="1:15">
       <c r="A86" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="M86" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="O86" s="17" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
     </row>
     <row r="87" spans="1:15">
       <c r="A87" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B87" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="M87" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="O87" s="17" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="88" spans="1:15">
       <c r="A88" t="s">
+        <v>298</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="M88" t="s">
+        <v>300</v>
+      </c>
+      <c r="O88" s="17" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15">
+      <c r="A89" t="s">
         <v>302</v>
       </c>
-      <c r="B88" s="7" t="s">
+      <c r="B89" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="M88" t="s">
+      <c r="M89" t="s">
         <v>304</v>
       </c>
-      <c r="O88" s="17" t="s">
+      <c r="O89" s="17" t="s">
         <v>305</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15">
-      <c r="A90" t="s">
-        <v>306</v>
-      </c>
-      <c r="B90" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="M90" t="s">
-        <v>308</v>
-      </c>
-      <c r="O90" s="17" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="91" spans="1:15">
       <c r="A91" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="M91" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="O91" s="17" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="92" spans="1:15">
       <c r="A92" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="M92" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="O92" s="17" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
     </row>
     <row r="93" spans="1:15">
       <c r="A93" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="O93" t="s">
-        <v>320</v>
+        <v>315</v>
+      </c>
+      <c r="M93" t="s">
+        <v>316</v>
+      </c>
+      <c r="O93" s="17" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="94" spans="1:15">
       <c r="A94" t="s">
+        <v>318</v>
+      </c>
+      <c r="B94" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="O94" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="95" spans="1:15">
+      <c r="A95" t="s">
         <v>321</v>
       </c>
-      <c r="B94" s="7" t="s">
+      <c r="B95" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="O94" t="s">
+      <c r="O95" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="95" spans="1:15">
-      <c r="B95" s="7"/>
-    </row>
     <row r="96" spans="1:15">
-      <c r="A96" s="3" t="s">
+      <c r="B96" s="7"/>
+    </row>
+    <row r="97" spans="1:15">
+      <c r="A97" s="3" t="s">
         <v>324</v>
       </c>
-      <c r="B96" s="7" t="s">
+      <c r="B97" s="7" t="s">
         <v>325</v>
       </c>
-      <c r="M96" s="3" t="s">
+      <c r="M97" s="3" t="s">
         <v>326</v>
       </c>
-      <c r="O96" t="s">
+      <c r="O97" t="s">
         <v>327</v>
-      </c>
-    </row>
-    <row r="97" spans="1:15">
-      <c r="A97" t="s">
-        <v>328</v>
-      </c>
-      <c r="B97" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="M97" t="s">
-        <v>330</v>
-      </c>
-      <c r="O97" s="17" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="98" spans="1:15">
       <c r="A98" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="M98" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="O98" s="17" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="99" spans="1:15">
       <c r="A99" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="M99" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="O99" s="17" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="100" spans="1:15">
       <c r="A100" t="s">
+        <v>336</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="M100" t="s">
+        <v>338</v>
+      </c>
+      <c r="O100" s="17" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15">
+      <c r="A101" t="s">
         <v>340</v>
       </c>
-      <c r="B100" s="7" t="s">
+      <c r="B101" s="7" t="s">
         <v>333</v>
       </c>
-      <c r="M100" t="s">
+      <c r="M101" t="s">
         <v>341</v>
       </c>
-      <c r="O100" s="17" t="s">
+      <c r="O101" s="17" t="s">
         <v>342</v>
-      </c>
-    </row>
-    <row r="102" spans="1:15">
-      <c r="A102" t="s">
-        <v>343</v>
-      </c>
-      <c r="B102" s="7" t="s">
-        <v>344</v>
-      </c>
-      <c r="M102" t="s">
-        <v>345</v>
-      </c>
-      <c r="O102" s="17" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="103" spans="1:15">
       <c r="A103" t="s">
+        <v>343</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="M103" t="s">
+        <v>345</v>
+      </c>
+      <c r="O103" s="17" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15">
+      <c r="A104" t="s">
         <v>347</v>
       </c>
-      <c r="B103" s="7" t="s">
+      <c r="B104" s="7" t="s">
         <v>348</v>
       </c>
-      <c r="M103" t="s">
+      <c r="M104" t="s">
         <v>349</v>
       </c>
-      <c r="O103" s="17" t="s">
+      <c r="O104" s="17" t="s">
         <v>350</v>
-      </c>
-    </row>
-    <row r="105" spans="1:15">
-      <c r="A105" t="s">
-        <v>351</v>
-      </c>
-      <c r="B105" t="s">
-        <v>352</v>
-      </c>
-      <c r="M105" t="s">
-        <v>353</v>
-      </c>
-      <c r="O105" s="17" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="106" spans="1:15">
       <c r="A106" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="B106" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="M106" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="O106" s="17" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
     </row>
     <row r="107" spans="1:15">
       <c r="A107" t="s">
+        <v>355</v>
+      </c>
+      <c r="B107" t="s">
+        <v>356</v>
+      </c>
+      <c r="M107" t="s">
+        <v>357</v>
+      </c>
+      <c r="O107" s="17" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15">
+      <c r="A108" t="s">
         <v>359</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>360</v>
       </c>
-      <c r="M107" t="s">
+      <c r="M108" t="s">
         <v>361</v>
       </c>
-      <c r="O107" s="17" t="s">
+      <c r="O108" s="17" t="s">
         <v>362</v>
-      </c>
-    </row>
-    <row r="109" spans="1:15">
-      <c r="A109" t="s">
-        <v>363</v>
-      </c>
-      <c r="B109" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="M109" t="s">
-        <v>365</v>
-      </c>
-      <c r="O109" s="17" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="110" spans="1:15">
       <c r="A110" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="M110" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="O110" s="17" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="111" spans="1:15">
       <c r="A111" t="s">
+        <v>367</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>368</v>
+      </c>
+      <c r="M111" t="s">
+        <v>369</v>
+      </c>
+      <c r="O111" s="17" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="112" spans="1:15">
+      <c r="A112" t="s">
         <v>371</v>
       </c>
-      <c r="B111" s="7" t="s">
+      <c r="B112" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="M111" t="s">
+      <c r="M112" t="s">
         <v>373</v>
       </c>
-      <c r="O111" s="17" t="s">
+      <c r="O112" s="17" t="s">
         <v>374</v>
-      </c>
-    </row>
-    <row r="113" spans="1:15">
-      <c r="A113" t="s">
-        <v>375</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>376</v>
-      </c>
-      <c r="M113" t="s">
-        <v>377</v>
-      </c>
-      <c r="O113" s="17" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="114" spans="1:15">
       <c r="A114" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="B114" s="7" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="M114" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="O114" s="17" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
     </row>
     <row r="115" spans="1:15">
       <c r="A115" t="s">
+        <v>379</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>380</v>
+      </c>
+      <c r="M115" t="s">
+        <v>381</v>
+      </c>
+      <c r="O115" s="17" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="116" spans="1:15">
+      <c r="A116" t="s">
         <v>383</v>
       </c>
-      <c r="B115" s="7" t="s">
+      <c r="B116" s="7" t="s">
         <v>384</v>
       </c>
-      <c r="M115" t="s">
+      <c r="M116" t="s">
         <v>385</v>
       </c>
-      <c r="O115" s="17" t="s">
+      <c r="O116" s="17" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="117" spans="1:15">
-      <c r="A117" t="s">
+    <row r="118" spans="1:15">
+      <c r="A118" t="s">
         <v>387</v>
       </c>
-      <c r="B117" s="7" t="s">
+      <c r="B118" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="M117" t="s">
+      <c r="M118" t="s">
         <v>389</v>
       </c>
-      <c r="O117" s="17" t="s">
+      <c r="O118" s="17" t="s">
         <v>390</v>
-      </c>
-    </row>
-    <row r="119" spans="1:15">
-      <c r="A119" t="s">
-        <v>391</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>392</v>
-      </c>
-      <c r="M119" t="s">
-        <v>393</v>
-      </c>
-      <c r="O119" s="17" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="120" spans="1:15">
       <c r="A120" t="s">
+        <v>391</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="M120" t="s">
+        <v>393</v>
+      </c>
+      <c r="O120" s="17" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="121" spans="1:15">
+      <c r="A121" t="s">
         <v>395</v>
       </c>
-      <c r="B120" s="7" t="s">
+      <c r="B121" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="M120" t="s">
+      <c r="M121" t="s">
         <v>397</v>
       </c>
-      <c r="O120" s="17" t="s">
+      <c r="O121" s="17" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="122" spans="1:15">
-      <c r="A122" t="s">
+    <row r="123" spans="1:15">
+      <c r="A123" t="s">
         <v>399</v>
       </c>
-      <c r="B122" t="s">
+      <c r="B123" t="s">
         <v>400</v>
       </c>
-      <c r="M122" t="s">
+      <c r="M123" t="s">
         <v>401</v>
       </c>
-      <c r="O122" s="17" t="s">
+      <c r="O123" s="17" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="123" spans="1:15">
-      <c r="O123" s="17"/>
-    </row>
     <row r="124" spans="1:15">
-      <c r="A124" s="3" t="s">
+      <c r="O124" s="17"/>
+    </row>
+    <row r="125" spans="1:15">
+      <c r="A125" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B125" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="M124" s="3" t="s">
+      <c r="M125" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="O124" t="s">
+      <c r="O125" t="s">
         <v>405</v>
-      </c>
-    </row>
-    <row r="125" spans="1:15">
-      <c r="A125" t="s">
-        <v>406</v>
-      </c>
-      <c r="B125" t="s">
-        <v>407</v>
-      </c>
-      <c r="M125" t="s">
-        <v>408</v>
-      </c>
-      <c r="O125" s="17" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="126" spans="1:15">
       <c r="A126" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B126" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="M126" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="O126" s="17" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="127" spans="1:15">
       <c r="A127" t="s">
-        <v>413</v>
-      </c>
-      <c r="B127" s="3" t="s">
-        <v>414</v>
+        <v>409</v>
+      </c>
+      <c r="B127" t="s">
+        <v>410</v>
       </c>
       <c r="M127" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="O127" s="17" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="128" spans="1:15">
       <c r="A128" t="s">
-        <v>416</v>
-      </c>
-      <c r="B128" t="s">
-        <v>417</v>
+        <v>413</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>414</v>
       </c>
       <c r="M128" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="O128" s="17" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="129" spans="1:15">
       <c r="A129" t="s">
+        <v>416</v>
+      </c>
+      <c r="B129" t="s">
+        <v>417</v>
+      </c>
+      <c r="M129" t="s">
+        <v>417</v>
+      </c>
+      <c r="O129" s="17" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="130" spans="1:15">
+      <c r="A130" t="s">
         <v>419</v>
       </c>
-      <c r="B129" t="s">
+      <c r="B130" t="s">
         <v>420</v>
       </c>
-      <c r="M129" t="s">
+      <c r="M130" t="s">
         <v>420</v>
       </c>
-      <c r="O129" s="17" t="s">
+      <c r="O130" s="17" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="130" spans="1:15" ht="21.75" customHeight="1">
-      <c r="A130" t="s">
+    <row r="131" spans="1:15" ht="21.75" customHeight="1">
+      <c r="A131" t="s">
         <v>421</v>
-      </c>
-      <c r="B130" s="3" t="s">
-        <v>422</v>
-      </c>
-      <c r="M130" t="s">
-        <v>423</v>
-      </c>
-      <c r="O130" s="17" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="131" spans="1:15">
-      <c r="A131" t="s">
-        <v>424</v>
       </c>
       <c r="B131" s="3" t="s">
         <v>422</v>
       </c>
       <c r="M131" t="s">
+        <v>423</v>
+      </c>
+      <c r="O131" s="17" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="132" spans="1:15">
+      <c r="A132" t="s">
+        <v>424</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="M132" t="s">
         <v>425</v>
       </c>
-      <c r="O131" s="17" t="s">
+      <c r="O132" s="17" t="s">
         <v>425</v>
-      </c>
-    </row>
-    <row r="133" spans="1:15">
-      <c r="A133" t="s">
-        <v>426</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="M133" t="s">
-        <v>428</v>
-      </c>
-      <c r="O133" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="134" spans="1:15">
       <c r="A134" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="M134" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="O134" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="135" spans="1:15">
       <c r="A135" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="M135" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="O135" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="136" spans="1:15">
       <c r="A136" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="M136" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="O136" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="137" spans="1:15">
       <c r="A137" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="M137" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="O137" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
     </row>
     <row r="138" spans="1:15">
       <c r="A138" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="M138" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="O138" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="139" spans="1:15" ht="409.5">
+    <row r="139" spans="1:15">
       <c r="A139" t="s">
+        <v>444</v>
+      </c>
+      <c r="B139" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="M139" t="s">
+        <v>446</v>
+      </c>
+      <c r="O139" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="140" spans="1:15" ht="409.5">
+      <c r="A140" t="s">
         <v>447</v>
       </c>
-      <c r="B139" s="5" t="s">
+      <c r="B140" s="5" t="s">
         <v>448</v>
       </c>
-      <c r="M139" s="5" t="s">
+      <c r="M140" s="5" t="s">
         <v>449</v>
       </c>
-      <c r="O139" s="6" t="s">
+      <c r="O140" s="6" t="s">
         <v>450</v>
-      </c>
-    </row>
-    <row r="141" spans="1:15">
-      <c r="A141" t="s">
-        <v>451</v>
-      </c>
-      <c r="B141" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="M141" t="s">
-        <v>453</v>
-      </c>
-      <c r="O141" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="142" spans="1:15">
       <c r="A142" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="M142" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="O142" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="143" spans="1:15">
       <c r="A143" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="M143" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="O143" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="144" spans="1:15">
       <c r="A144" t="s">
+        <v>459</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="M144" t="s">
+        <v>461</v>
+      </c>
+      <c r="O144" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="145" spans="1:15">
+      <c r="A145" t="s">
         <v>463</v>
       </c>
-      <c r="B144" s="3" t="s">
+      <c r="B145" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="M144" t="s">
+      <c r="M145" t="s">
         <v>465</v>
       </c>
-      <c r="O144" t="s">
+      <c r="O145" t="s">
         <v>466</v>
-      </c>
-    </row>
-    <row r="146" spans="1:15">
-      <c r="A146" t="s">
-        <v>467</v>
-      </c>
-      <c r="B146" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="M146" t="s">
-        <v>469</v>
-      </c>
-      <c r="O146" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="147" spans="1:15">
       <c r="A147" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="M147" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="O147" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
     </row>
     <row r="148" spans="1:15">
       <c r="A148" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="M148" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="O148" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
     </row>
     <row r="149" spans="1:15">
       <c r="A149" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="M149" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="O149" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
     </row>
     <row r="150" spans="1:15">
       <c r="A150" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="M150" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="O150" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
     </row>
     <row r="151" spans="1:15">
       <c r="A151" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="M151" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="O151" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
     </row>
     <row r="152" spans="1:15">
       <c r="A152" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="M152" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="O152" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
     </row>
     <row r="153" spans="1:15">
       <c r="A153" t="s">
+        <v>491</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="M153" t="s">
+        <v>493</v>
+      </c>
+      <c r="O153" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="154" spans="1:15">
+      <c r="A154" t="s">
         <v>495</v>
       </c>
-      <c r="B153" s="3" t="s">
+      <c r="B154" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="M153" t="s">
+      <c r="M154" t="s">
         <v>497</v>
       </c>
-      <c r="O153" t="s">
+      <c r="O154" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="157" spans="1:15">
-      <c r="A157" t="s">
+    <row r="158" spans="1:15">
+      <c r="A158" t="s">
         <v>499</v>
       </c>
-      <c r="B157" s="3" t="s">
+      <c r="B158" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="M157" s="3" t="s">
+      <c r="M158" s="3" t="s">
         <v>501</v>
       </c>
-      <c r="O157" s="17" t="s">
+      <c r="O158" s="17" t="s">
         <v>502</v>
-      </c>
-    </row>
-    <row r="159" spans="1:15">
-      <c r="A159" t="s">
-        <v>503</v>
-      </c>
-      <c r="B159" s="7" t="s">
-        <v>504</v>
-      </c>
-      <c r="M159" t="s">
-        <v>505</v>
-      </c>
-      <c r="O159" s="17" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="160" spans="1:15">
       <c r="A160" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="B160" s="7" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="M160" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="O160" s="17" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
     </row>
     <row r="161" spans="1:15">
       <c r="A161" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="M161" t="s">
-        <v>513</v>
-      </c>
-      <c r="O161" t="s">
-        <v>514</v>
+        <v>509</v>
+      </c>
+      <c r="O161" s="17" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="162" spans="1:15">
       <c r="A162" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="M162" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="O162" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
     </row>
     <row r="163" spans="1:15">
       <c r="A163" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>520</v>
-      </c>
-      <c r="M163" s="3" t="s">
-        <v>521</v>
+        <v>516</v>
+      </c>
+      <c r="M163" t="s">
+        <v>517</v>
       </c>
       <c r="O163" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
     </row>
     <row r="164" spans="1:15">
       <c r="A164" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="B164" s="7" t="s">
-        <v>524</v>
-      </c>
-      <c r="M164" t="s">
-        <v>525</v>
+        <v>520</v>
+      </c>
+      <c r="M164" s="3" t="s">
+        <v>521</v>
       </c>
       <c r="O164" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
     </row>
     <row r="165" spans="1:15">
       <c r="A165" t="s">
+        <v>523</v>
+      </c>
+      <c r="B165" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="M165" t="s">
+        <v>525</v>
+      </c>
+      <c r="O165" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="166" spans="1:15">
+      <c r="A166" t="s">
         <v>527</v>
       </c>
-      <c r="B165" s="7" t="s">
+      <c r="B166" s="7" t="s">
         <v>528</v>
       </c>
-      <c r="M165" t="s">
+      <c r="M166" t="s">
         <v>529</v>
       </c>
-      <c r="O165" t="s">
+      <c r="O166" t="s">
         <v>530</v>
-      </c>
-    </row>
-    <row r="167" spans="1:15">
-      <c r="A167" t="s">
-        <v>531</v>
-      </c>
-      <c r="B167" s="7" t="s">
-        <v>531</v>
-      </c>
-      <c r="M167" t="s">
-        <v>532</v>
-      </c>
-      <c r="O167" s="17" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="168" spans="1:15">
       <c r="A168" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B168" s="7" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="M168" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="O168" s="17" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
     </row>
     <row r="169" spans="1:15">
       <c r="A169" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="M169" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="O169" s="17" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="170" spans="1:15">
       <c r="A170" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="M170" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="O170" s="17" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="171" spans="1:15">
       <c r="A171" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="M171" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="O171" s="17" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
     </row>
     <row r="172" spans="1:15">
       <c r="A172" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="B172" s="7" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="M172" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="O172" s="17" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="173" spans="1:15">
       <c r="A173" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B173" s="7" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="M173" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="O173" s="17" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="174" spans="1:15">
       <c r="A174" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="M174" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="O174" s="17" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="175" spans="1:15">
       <c r="A175" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="M175" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="O175" s="17" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="176" spans="1:15">
       <c r="A176" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="B176" s="7" t="s">
         <v>557</v>
       </c>
       <c r="M176" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="O176" s="17" t="s">
         <v>559</v>
@@ -21439,1174 +21448,1176 @@
     </row>
     <row r="177" spans="1:15">
       <c r="A177" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="B177" s="7" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="M177" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="O177" s="17" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="178" spans="1:15">
       <c r="A178" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B178" s="7" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="M178" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="O178" s="17" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
     </row>
     <row r="179" spans="1:15">
       <c r="A179" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="M179" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="O179" s="17" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
     </row>
     <row r="180" spans="1:15">
       <c r="A180" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B180" s="7" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="M180" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="O180" s="17" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="181" spans="1:15">
       <c r="A181" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="M181" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="O181" s="17" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="182" spans="1:15">
       <c r="A182" t="s">
+        <v>578</v>
+      </c>
+      <c r="B182" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="M182" t="s">
+        <v>580</v>
+      </c>
+      <c r="O182" s="17" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="183" spans="1:15">
+      <c r="A183" t="s">
         <v>582</v>
       </c>
-      <c r="B182" s="7" t="s">
+      <c r="B183" s="7" t="s">
         <v>583</v>
       </c>
-      <c r="M182" t="s">
+      <c r="M183" t="s">
         <v>584</v>
       </c>
-      <c r="O182" t="s">
+      <c r="O183" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="185" spans="1:15">
-      <c r="A185" t="s">
+    <row r="186" spans="1:15">
+      <c r="A186" t="s">
         <v>586</v>
       </c>
-      <c r="M185" s="3" t="s">
+      <c r="M186" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="O185" t="s">
+      <c r="O186" t="s">
         <v>588</v>
-      </c>
-    </row>
-    <row r="187" spans="1:15">
-      <c r="A187" t="s">
-        <v>589</v>
-      </c>
-      <c r="B187" s="7" t="s">
-        <v>590</v>
-      </c>
-      <c r="M187" t="s">
-        <v>591</v>
-      </c>
-      <c r="O187" s="17" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="188" spans="1:15">
       <c r="A188" t="s">
+        <v>589</v>
+      </c>
+      <c r="B188" s="7" t="s">
+        <v>590</v>
+      </c>
+      <c r="M188" t="s">
+        <v>591</v>
+      </c>
+      <c r="O188" s="17" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="189" spans="1:15">
+      <c r="A189" t="s">
         <v>593</v>
       </c>
-      <c r="B188" s="7" t="s">
+      <c r="B189" s="7" t="s">
         <v>594</v>
       </c>
-      <c r="M188" t="s">
+      <c r="M189" t="s">
         <v>595</v>
       </c>
-      <c r="O188" s="17" t="s">
+      <c r="O189" s="17" t="s">
         <v>596</v>
-      </c>
-    </row>
-    <row r="190" spans="1:15">
-      <c r="A190" t="s">
-        <v>597</v>
-      </c>
-      <c r="B190" s="7" t="s">
-        <v>598</v>
-      </c>
-      <c r="M190" t="s">
-        <v>599</v>
-      </c>
-      <c r="O190" s="17" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="191" spans="1:15">
       <c r="A191" t="s">
+        <v>597</v>
+      </c>
+      <c r="B191" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="M191" t="s">
+        <v>599</v>
+      </c>
+      <c r="O191" s="17" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="192" spans="1:15">
+      <c r="A192" t="s">
         <v>601</v>
       </c>
-      <c r="B191" s="7" t="s">
+      <c r="B192" s="7" t="s">
         <v>602</v>
       </c>
-      <c r="M191" t="s">
+      <c r="M192" t="s">
         <v>603</v>
       </c>
-      <c r="O191" s="17" t="s">
+      <c r="O192" s="17" t="s">
         <v>604</v>
-      </c>
-    </row>
-    <row r="193" spans="1:15">
-      <c r="A193" t="s">
-        <v>605</v>
-      </c>
-      <c r="B193" s="7" t="s">
-        <v>606</v>
-      </c>
-      <c r="M193" t="s">
-        <v>607</v>
-      </c>
-      <c r="O193" s="17" t="s">
-        <v>608</v>
       </c>
     </row>
     <row r="194" spans="1:15">
       <c r="A194" t="s">
+        <v>605</v>
+      </c>
+      <c r="B194" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="M194" t="s">
+        <v>607</v>
+      </c>
+      <c r="O194" s="17" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="195" spans="1:15">
+      <c r="A195" t="s">
         <v>609</v>
       </c>
-      <c r="B194" s="7" t="s">
+      <c r="B195" s="7" t="s">
         <v>610</v>
       </c>
-      <c r="M194" t="s">
+      <c r="M195" t="s">
         <v>611</v>
       </c>
-      <c r="O194" s="17" t="s">
+      <c r="O195" s="17" t="s">
         <v>612</v>
-      </c>
-    </row>
-    <row r="196" spans="1:15">
-      <c r="A196" t="s">
-        <v>613</v>
-      </c>
-      <c r="B196" s="7" t="s">
-        <v>613</v>
-      </c>
-      <c r="M196" t="s">
-        <v>614</v>
-      </c>
-      <c r="O196" s="17" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="197" spans="1:15">
       <c r="A197" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>616</v>
+        <v>613</v>
       </c>
       <c r="M197" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="O197" s="17" t="s">
-        <v>618</v>
+        <v>615</v>
       </c>
     </row>
     <row r="198" spans="1:15">
       <c r="A198" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B198" s="7" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="M198" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="O198" s="17" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
     </row>
     <row r="199" spans="1:15">
       <c r="A199" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="M199" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="O199" s="17" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
     </row>
     <row r="200" spans="1:15">
       <c r="A200" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B200" s="7" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="M200" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="O200" s="17" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
     </row>
     <row r="201" spans="1:15">
       <c r="A201" t="s">
+        <v>626</v>
+      </c>
+      <c r="B201" s="7" t="s">
+        <v>626</v>
+      </c>
+      <c r="M201" t="s">
+        <v>627</v>
+      </c>
+      <c r="O201" s="17" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="202" spans="1:15">
+      <c r="A202" t="s">
         <v>629</v>
       </c>
-      <c r="B201" s="7" t="s">
+      <c r="B202" s="7" t="s">
         <v>630</v>
       </c>
-      <c r="M201" t="s">
+      <c r="M202" t="s">
         <v>631</v>
       </c>
-      <c r="O201" s="17" t="s">
+      <c r="O202" s="17" t="s">
         <v>632</v>
-      </c>
-    </row>
-    <row r="205" spans="1:15">
-      <c r="A205" t="s">
-        <v>633</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="M205" t="s">
-        <v>635</v>
-      </c>
-      <c r="O205" t="s">
-        <v>636</v>
       </c>
     </row>
     <row r="206" spans="1:15">
       <c r="A206" t="s">
-        <v>637</v>
-      </c>
-      <c r="B206" s="7" t="s">
-        <v>638</v>
+        <v>633</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>634</v>
       </c>
       <c r="M206" t="s">
-        <v>639</v>
-      </c>
-      <c r="O206" s="17" t="s">
-        <v>640</v>
+        <v>635</v>
+      </c>
+      <c r="O206" t="s">
+        <v>636</v>
       </c>
     </row>
     <row r="207" spans="1:15">
       <c r="A207" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="M207" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="O207" s="17" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="208" spans="1:15">
       <c r="A208" t="s">
+        <v>641</v>
+      </c>
+      <c r="B208" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="M208" t="s">
+        <v>643</v>
+      </c>
+      <c r="O208" s="17" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="209" spans="1:15">
+      <c r="A209" t="s">
         <v>645</v>
       </c>
-      <c r="B208" s="7" t="s">
+      <c r="B209" s="7" t="s">
         <v>646</v>
       </c>
-      <c r="M208" t="s">
+      <c r="M209" t="s">
         <v>647</v>
       </c>
-      <c r="O208" s="17" t="s">
+      <c r="O209" s="17" t="s">
         <v>648</v>
-      </c>
-    </row>
-    <row r="210" spans="1:15">
-      <c r="A210" t="s">
-        <v>649</v>
-      </c>
-      <c r="B210" s="7" t="s">
-        <v>650</v>
-      </c>
-      <c r="M210" t="s">
-        <v>651</v>
-      </c>
-      <c r="O210" s="17" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="211" spans="1:15">
       <c r="A211" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="M211" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="O211" s="17" t="s">
-        <v>327</v>
+        <v>652</v>
       </c>
     </row>
     <row r="212" spans="1:15">
       <c r="A212" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B212" s="7" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="M212" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="O212" s="17" t="s">
-        <v>659</v>
+        <v>327</v>
       </c>
     </row>
     <row r="213" spans="1:15">
       <c r="A213" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="B213" s="7" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="M213" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="O213" s="17" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
     </row>
     <row r="214" spans="1:15">
       <c r="A214" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="B214" s="7" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="M214" t="s">
-        <v>666</v>
-      </c>
-      <c r="O214" t="s">
-        <v>667</v>
+        <v>662</v>
+      </c>
+      <c r="O214" s="17" t="s">
+        <v>663</v>
       </c>
     </row>
     <row r="215" spans="1:15">
       <c r="A215" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="B215" s="7" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="M215" t="s">
-        <v>670</v>
-      </c>
-      <c r="O215" s="17" t="s">
-        <v>671</v>
+        <v>666</v>
+      </c>
+      <c r="O215" t="s">
+        <v>667</v>
       </c>
     </row>
     <row r="216" spans="1:15">
       <c r="A216" t="s">
+        <v>668</v>
+      </c>
+      <c r="B216" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="M216" t="s">
+        <v>670</v>
+      </c>
+      <c r="O216" s="17" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="217" spans="1:15">
+      <c r="A217" t="s">
         <v>672</v>
       </c>
-      <c r="B216" s="7" t="s">
+      <c r="B217" s="7" t="s">
         <v>673</v>
       </c>
-      <c r="M216" t="s">
+      <c r="M217" t="s">
         <v>674</v>
       </c>
-      <c r="O216" s="17" t="s">
+      <c r="O217" s="17" t="s">
         <v>675</v>
-      </c>
-    </row>
-    <row r="218" spans="1:15">
-      <c r="A218" t="s">
-        <v>676</v>
-      </c>
-      <c r="B218" s="7" t="s">
-        <v>677</v>
-      </c>
-      <c r="M218" t="s">
-        <v>678</v>
-      </c>
-      <c r="O218" s="17" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="219" spans="1:15">
       <c r="A219" t="s">
+        <v>676</v>
+      </c>
+      <c r="B219" s="7" t="s">
+        <v>677</v>
+      </c>
+      <c r="M219" t="s">
+        <v>678</v>
+      </c>
+      <c r="O219" s="17" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="220" spans="1:15">
+      <c r="A220" t="s">
         <v>680</v>
       </c>
-      <c r="B219" s="7" t="s">
+      <c r="B220" s="7" t="s">
         <v>681</v>
       </c>
-      <c r="M219" t="s">
+      <c r="M220" t="s">
         <v>682</v>
       </c>
-      <c r="O219" s="17" t="s">
+      <c r="O220" s="17" t="s">
         <v>683</v>
-      </c>
-    </row>
-    <row r="221" spans="1:15">
-      <c r="A221" t="s">
-        <v>684</v>
-      </c>
-      <c r="B221" s="7" t="s">
-        <v>685</v>
-      </c>
-      <c r="M221" t="s">
-        <v>686</v>
-      </c>
-      <c r="O221" s="17" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="222" spans="1:15">
       <c r="A222" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="B222" s="7" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="M222" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="O222" s="17" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
     </row>
     <row r="223" spans="1:15">
       <c r="A223" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="B223" s="7" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="M223" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="O223" s="17" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
     </row>
     <row r="224" spans="1:15">
       <c r="A224" t="s">
+        <v>692</v>
+      </c>
+      <c r="B224" s="7" t="s">
+        <v>693</v>
+      </c>
+      <c r="M224" t="s">
+        <v>694</v>
+      </c>
+      <c r="O224" s="17" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="225" spans="1:15">
+      <c r="A225" t="s">
         <v>696</v>
       </c>
-      <c r="B224" s="7" t="s">
+      <c r="B225" s="7" t="s">
         <v>697</v>
       </c>
-      <c r="M224" t="s">
+      <c r="M225" t="s">
         <v>698</v>
       </c>
-      <c r="O224" s="17" t="s">
+      <c r="O225" s="17" t="s">
         <v>699</v>
       </c>
     </row>
-    <row r="226" spans="1:15">
-      <c r="A226" t="s">
+    <row r="227" spans="1:15">
+      <c r="A227" t="s">
         <v>700</v>
       </c>
-      <c r="B226" s="7" t="s">
+      <c r="B227" s="7" t="s">
         <v>701</v>
       </c>
-      <c r="M226" t="s">
+      <c r="M227" t="s">
         <v>702</v>
       </c>
-      <c r="O226" s="17" t="s">
+      <c r="O227" s="17" t="s">
         <v>703</v>
       </c>
     </row>
-    <row r="228" spans="1:15">
-      <c r="A228" t="s">
+    <row r="229" spans="1:15">
+      <c r="A229" t="s">
         <v>704</v>
       </c>
-      <c r="B228" s="3" t="s">
+      <c r="B229" s="3" t="s">
         <v>705</v>
       </c>
-      <c r="M228" t="s">
+      <c r="M229" t="s">
         <v>706</v>
       </c>
-      <c r="O228" t="s">
+      <c r="O229" t="s">
         <v>707</v>
-      </c>
-    </row>
-    <row r="230" spans="1:15">
-      <c r="A230" t="s">
-        <v>708</v>
-      </c>
-      <c r="B230" s="7" t="s">
-        <v>709</v>
-      </c>
-      <c r="M230" t="s">
-        <v>710</v>
-      </c>
-      <c r="O230" s="4" t="s">
-        <v>711</v>
       </c>
     </row>
     <row r="231" spans="1:15">
       <c r="A231" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="B231" s="7" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="M231" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="O231" s="4" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
     </row>
     <row r="232" spans="1:15">
       <c r="A232" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="B232" s="7" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="M232" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="O232" s="4" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
     </row>
     <row r="233" spans="1:15">
       <c r="A233" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="B233" s="7" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="M233" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="O233" s="4" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
     </row>
     <row r="234" spans="1:15">
       <c r="A234" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="B234" s="7" t="s">
-        <v>725</v>
+        <v>721</v>
       </c>
       <c r="M234" t="s">
-        <v>726</v>
+        <v>722</v>
       </c>
       <c r="O234" s="4" t="s">
-        <v>727</v>
+        <v>723</v>
       </c>
     </row>
     <row r="235" spans="1:15">
       <c r="A235" t="s">
-        <v>728</v>
+        <v>724</v>
       </c>
       <c r="B235" s="7" t="s">
-        <v>729</v>
+        <v>725</v>
       </c>
       <c r="M235" t="s">
-        <v>730</v>
+        <v>726</v>
       </c>
       <c r="O235" s="4" t="s">
-        <v>731</v>
+        <v>727</v>
       </c>
     </row>
     <row r="236" spans="1:15">
       <c r="A236" t="s">
-        <v>732</v>
+        <v>728</v>
       </c>
       <c r="B236" s="7" t="s">
-        <v>733</v>
+        <v>729</v>
       </c>
       <c r="M236" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="O236" s="4" t="s">
-        <v>735</v>
+        <v>731</v>
       </c>
     </row>
     <row r="237" spans="1:15">
       <c r="A237" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="M237" t="s">
-        <v>738</v>
+        <v>734</v>
       </c>
       <c r="O237" s="4" t="s">
-        <v>739</v>
+        <v>735</v>
       </c>
     </row>
     <row r="238" spans="1:15">
       <c r="A238" t="s">
-        <v>740</v>
+        <v>736</v>
       </c>
       <c r="B238" s="7" t="s">
-        <v>741</v>
+        <v>737</v>
       </c>
       <c r="M238" t="s">
-        <v>742</v>
+        <v>738</v>
       </c>
       <c r="O238" s="4" t="s">
-        <v>743</v>
+        <v>739</v>
       </c>
     </row>
     <row r="239" spans="1:15">
       <c r="A239" t="s">
-        <v>744</v>
+        <v>740</v>
       </c>
       <c r="B239" s="7" t="s">
-        <v>745</v>
+        <v>741</v>
       </c>
       <c r="M239" t="s">
-        <v>746</v>
+        <v>742</v>
       </c>
       <c r="O239" s="4" t="s">
-        <v>747</v>
+        <v>743</v>
       </c>
     </row>
     <row r="240" spans="1:15">
       <c r="A240" t="s">
-        <v>748</v>
+        <v>744</v>
       </c>
       <c r="B240" s="7" t="s">
-        <v>749</v>
+        <v>745</v>
       </c>
       <c r="M240" t="s">
-        <v>750</v>
+        <v>746</v>
       </c>
       <c r="O240" s="4" t="s">
-        <v>751</v>
+        <v>747</v>
       </c>
     </row>
     <row r="241" spans="1:15">
       <c r="A241" t="s">
-        <v>752</v>
+        <v>748</v>
       </c>
       <c r="B241" s="7" t="s">
-        <v>753</v>
+        <v>749</v>
       </c>
       <c r="M241" t="s">
-        <v>754</v>
+        <v>750</v>
       </c>
       <c r="O241" s="4" t="s">
-        <v>755</v>
+        <v>751</v>
       </c>
     </row>
     <row r="242" spans="1:15">
       <c r="A242" t="s">
-        <v>756</v>
+        <v>752</v>
       </c>
       <c r="B242" s="7" t="s">
-        <v>757</v>
+        <v>753</v>
       </c>
       <c r="M242" t="s">
-        <v>758</v>
+        <v>754</v>
       </c>
       <c r="O242" s="4" t="s">
-        <v>759</v>
+        <v>755</v>
       </c>
     </row>
     <row r="243" spans="1:15">
       <c r="A243" t="s">
-        <v>760</v>
+        <v>756</v>
       </c>
       <c r="B243" s="7" t="s">
-        <v>761</v>
+        <v>757</v>
       </c>
       <c r="M243" t="s">
-        <v>762</v>
+        <v>758</v>
       </c>
       <c r="O243" s="4" t="s">
-        <v>763</v>
+        <v>759</v>
       </c>
     </row>
     <row r="244" spans="1:15">
       <c r="A244" t="s">
-        <v>764</v>
+        <v>760</v>
       </c>
       <c r="B244" s="7" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="M244" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="O244" s="4" t="s">
-        <v>767</v>
+        <v>763</v>
       </c>
     </row>
     <row r="245" spans="1:15">
       <c r="A245" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="B245" s="7" t="s">
-        <v>769</v>
+        <v>765</v>
       </c>
       <c r="M245" t="s">
-        <v>770</v>
+        <v>766</v>
       </c>
       <c r="O245" s="4" t="s">
-        <v>771</v>
+        <v>767</v>
       </c>
     </row>
     <row r="246" spans="1:15">
       <c r="A246" t="s">
-        <v>772</v>
+        <v>768</v>
       </c>
       <c r="B246" s="7" t="s">
-        <v>773</v>
+        <v>769</v>
       </c>
       <c r="M246" t="s">
-        <v>774</v>
+        <v>770</v>
       </c>
       <c r="O246" s="4" t="s">
-        <v>775</v>
+        <v>771</v>
       </c>
     </row>
     <row r="247" spans="1:15">
       <c r="A247" t="s">
-        <v>776</v>
+        <v>772</v>
       </c>
       <c r="B247" s="7" t="s">
-        <v>777</v>
+        <v>773</v>
       </c>
       <c r="M247" t="s">
-        <v>778</v>
+        <v>774</v>
       </c>
       <c r="O247" s="4" t="s">
-        <v>779</v>
+        <v>775</v>
       </c>
     </row>
     <row r="248" spans="1:15">
       <c r="A248" t="s">
+        <v>776</v>
+      </c>
+      <c r="B248" s="7" t="s">
+        <v>777</v>
+      </c>
+      <c r="M248" t="s">
+        <v>778</v>
+      </c>
+      <c r="O248" s="4" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="249" spans="1:15">
+      <c r="A249" t="s">
         <v>780</v>
       </c>
-      <c r="B248" s="7" t="s">
+      <c r="B249" s="7" t="s">
         <v>781</v>
       </c>
-      <c r="M248" t="s">
+      <c r="M249" t="s">
         <v>782</v>
       </c>
-      <c r="O248" s="4" t="s">
+      <c r="O249" s="4" t="s">
         <v>783</v>
-      </c>
-    </row>
-    <row r="250" spans="1:15">
-      <c r="A250" t="s">
-        <v>784</v>
-      </c>
-      <c r="B250" s="7" t="s">
-        <v>785</v>
-      </c>
-      <c r="M250" t="s">
-        <v>786</v>
-      </c>
-      <c r="O250" s="4" t="s">
-        <v>787</v>
       </c>
     </row>
     <row r="251" spans="1:15">
       <c r="A251" t="s">
-        <v>788</v>
+        <v>784</v>
       </c>
       <c r="B251" s="7" t="s">
-        <v>789</v>
+        <v>785</v>
       </c>
       <c r="M251" t="s">
-        <v>790</v>
+        <v>786</v>
       </c>
       <c r="O251" s="4" t="s">
-        <v>791</v>
+        <v>787</v>
       </c>
     </row>
     <row r="252" spans="1:15">
       <c r="A252" t="s">
+        <v>788</v>
+      </c>
+      <c r="B252" s="7" t="s">
+        <v>789</v>
+      </c>
+      <c r="M252" t="s">
+        <v>790</v>
+      </c>
+      <c r="O252" s="4" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="253" spans="1:15">
+      <c r="A253" t="s">
         <v>792</v>
       </c>
-      <c r="B252" s="7" t="s">
+      <c r="B253" s="7" t="s">
         <v>793</v>
       </c>
-      <c r="M252" t="s">
+      <c r="M253" t="s">
         <v>794</v>
       </c>
-      <c r="O252" s="4" t="s">
+      <c r="O253" s="4" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="254" spans="1:15">
-      <c r="A254" t="s">
+    <row r="255" spans="1:15">
+      <c r="A255" t="s">
         <v>796</v>
       </c>
-      <c r="B254" s="7" t="s">
+      <c r="B255" s="7" t="s">
         <v>797</v>
       </c>
-      <c r="M254" t="s">
+      <c r="M255" t="s">
         <v>798</v>
       </c>
-      <c r="O254" s="17" t="s">
+      <c r="O255" s="17" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="256" spans="1:15">
-      <c r="A256" t="s">
+    <row r="257" spans="1:15">
+      <c r="A257" t="s">
         <v>800</v>
       </c>
-      <c r="B256" s="7" t="s">
+      <c r="B257" s="7" t="s">
         <v>801</v>
       </c>
-      <c r="M256" t="s">
+      <c r="M257" t="s">
         <v>802</v>
       </c>
-      <c r="O256" s="17" t="s">
+      <c r="O257" s="17" t="s">
         <v>803</v>
-      </c>
-    </row>
-    <row r="258" spans="1:15">
-      <c r="A258" t="s">
-        <v>804</v>
-      </c>
-      <c r="B258" s="7" t="s">
-        <v>805</v>
-      </c>
-      <c r="M258" t="s">
-        <v>806</v>
-      </c>
-      <c r="O258" s="17" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="259" spans="1:15">
       <c r="A259" t="s">
-        <v>808</v>
+        <v>804</v>
       </c>
       <c r="B259" s="7" t="s">
-        <v>809</v>
+        <v>805</v>
       </c>
       <c r="M259" t="s">
-        <v>810</v>
+        <v>806</v>
       </c>
       <c r="O259" s="17" t="s">
-        <v>811</v>
+        <v>807</v>
       </c>
     </row>
     <row r="260" spans="1:15">
       <c r="A260" t="s">
-        <v>812</v>
+        <v>808</v>
       </c>
       <c r="B260" s="7" t="s">
-        <v>813</v>
+        <v>809</v>
       </c>
       <c r="M260" t="s">
-        <v>814</v>
+        <v>810</v>
       </c>
       <c r="O260" s="17" t="s">
-        <v>815</v>
+        <v>811</v>
       </c>
     </row>
     <row r="261" spans="1:15">
       <c r="A261" t="s">
-        <v>816</v>
+        <v>812</v>
       </c>
       <c r="B261" s="7" t="s">
-        <v>817</v>
+        <v>813</v>
       </c>
       <c r="M261" t="s">
-        <v>818</v>
+        <v>814</v>
       </c>
       <c r="O261" s="17" t="s">
-        <v>819</v>
+        <v>815</v>
       </c>
     </row>
     <row r="262" spans="1:15">
       <c r="A262" t="s">
+        <v>816</v>
+      </c>
+      <c r="B262" s="7" t="s">
+        <v>817</v>
+      </c>
+      <c r="M262" t="s">
+        <v>818</v>
+      </c>
+      <c r="O262" s="17" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="263" spans="1:15">
+      <c r="A263" t="s">
         <v>820</v>
       </c>
-      <c r="B262" s="7" t="s">
+      <c r="B263" s="7" t="s">
         <v>821</v>
       </c>
-      <c r="M262" t="s">
+      <c r="M263" t="s">
         <v>822</v>
       </c>
-      <c r="O262" s="17" t="s">
+      <c r="O263" s="17" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="263" spans="1:15">
-      <c r="B263" s="7"/>
-      <c r="O263" s="17"/>
-    </row>
     <row r="264" spans="1:15">
-      <c r="A264" s="19" t="s">
-        <v>5023</v>
-      </c>
       <c r="B264" s="7"/>
-      <c r="M264" s="3" t="s">
-        <v>824</v>
-      </c>
-      <c r="O264" s="3" t="s">
-        <v>825</v>
-      </c>
+      <c r="O264" s="17"/>
     </row>
     <row r="265" spans="1:15">
       <c r="A265" s="19" t="s">
-        <v>5024</v>
+        <v>5023</v>
       </c>
       <c r="B265" s="7"/>
       <c r="M265" s="3" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="O265" s="3" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="266" spans="1:15">
       <c r="A266" s="19" t="s">
-        <v>5025</v>
+        <v>5024</v>
       </c>
       <c r="B266" s="7"/>
       <c r="M266" s="3" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="O266" s="3" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
     </row>
     <row r="267" spans="1:15">
       <c r="A267" s="19" t="s">
-        <v>5026</v>
+        <v>5025</v>
       </c>
       <c r="B267" s="7"/>
       <c r="M267" s="3" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="O267" s="3" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
     </row>
     <row r="268" spans="1:15">
       <c r="A268" s="19" t="s">
-        <v>5027</v>
+        <v>5026</v>
       </c>
       <c r="B268" s="7"/>
       <c r="M268" s="3" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="O268" s="3" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="269" spans="1:15">
       <c r="A269" s="19" t="s">
-        <v>5028</v>
+        <v>5027</v>
       </c>
       <c r="B269" s="7"/>
       <c r="M269" s="3" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="O269" s="3" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="270" spans="1:15">
       <c r="A270" s="19" t="s">
-        <v>5029</v>
+        <v>5028</v>
       </c>
       <c r="B270" s="7"/>
       <c r="M270" s="3" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="O270" s="3" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="271" spans="1:15">
       <c r="A271" s="19" t="s">
-        <v>5030</v>
+        <v>5029</v>
       </c>
       <c r="B271" s="7"/>
       <c r="M271" s="3" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="O271" s="3" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
     </row>
     <row r="272" spans="1:15">
       <c r="A272" s="19" t="s">
-        <v>5031</v>
+        <v>5030</v>
       </c>
       <c r="B272" s="7"/>
       <c r="M272" s="3" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="O272" s="3" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
     </row>
     <row r="273" spans="1:15">
       <c r="A273" s="19" t="s">
-        <v>5032</v>
+        <v>5031</v>
       </c>
       <c r="B273" s="7"/>
       <c r="M273" s="3" t="s">
-        <v>826</v>
+        <v>832</v>
       </c>
       <c r="O273" s="3" t="s">
-        <v>827</v>
+        <v>833</v>
       </c>
     </row>
     <row r="274" spans="1:15">
       <c r="A274" s="19" t="s">
-        <v>5033</v>
+        <v>5032</v>
       </c>
       <c r="B274" s="7"/>
       <c r="M274" s="3" t="s">
-        <v>834</v>
+        <v>826</v>
       </c>
       <c r="O274" s="3" t="s">
-        <v>833</v>
+        <v>827</v>
       </c>
     </row>
     <row r="275" spans="1:15">
       <c r="A275" s="19" t="s">
-        <v>5034</v>
+        <v>5033</v>
       </c>
       <c r="B275" s="7"/>
       <c r="M275" s="3" t="s">
-        <v>826</v>
+        <v>834</v>
       </c>
       <c r="O275" s="3" t="s">
-        <v>827</v>
+        <v>833</v>
       </c>
     </row>
     <row r="276" spans="1:15">
       <c r="A276" s="19" t="s">
-        <v>5035</v>
+        <v>5034</v>
       </c>
       <c r="B276" s="7"/>
       <c r="M276" s="3" t="s">
-        <v>835</v>
+        <v>826</v>
       </c>
       <c r="O276" s="3" t="s">
-        <v>836</v>
+        <v>827</v>
       </c>
     </row>
     <row r="277" spans="1:15">
       <c r="A277" s="19" t="s">
-        <v>5036</v>
+        <v>5035</v>
       </c>
       <c r="B277" s="7"/>
       <c r="M277" s="3" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="O277" s="3" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
     </row>
     <row r="278" spans="1:15">
       <c r="A278" s="19" t="s">
-        <v>5037</v>
+        <v>5036</v>
       </c>
       <c r="B278" s="7"/>
       <c r="M278" s="3" t="s">
-        <v>835</v>
+        <v>830</v>
       </c>
       <c r="O278" s="3" t="s">
-        <v>836</v>
+        <v>831</v>
       </c>
     </row>
     <row r="279" spans="1:15">
       <c r="A279" s="19" t="s">
-        <v>5038</v>
+        <v>5037</v>
       </c>
       <c r="B279" s="7"/>
       <c r="M279" s="3" t="s">
-        <v>830</v>
+        <v>835</v>
       </c>
       <c r="O279" s="3" t="s">
-        <v>831</v>
+        <v>836</v>
       </c>
     </row>
     <row r="280" spans="1:15">
-      <c r="A280" s="3" t="s">
-        <v>837</v>
+      <c r="A280" s="19" t="s">
+        <v>5038</v>
       </c>
       <c r="B280" s="7"/>
       <c r="M280" s="3" t="s">
-        <v>838</v>
+        <v>830</v>
       </c>
       <c r="O280" s="3" t="s">
-        <v>839</v>
+        <v>831</v>
       </c>
     </row>
     <row r="281" spans="1:15">
       <c r="A281" s="3" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="B281" s="7"/>
       <c r="M281" s="3" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="O281" s="3" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
     </row>
     <row r="282" spans="1:15">
       <c r="A282" s="3" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="B282" s="7"/>
       <c r="M282" s="3" t="s">
-        <v>844</v>
-      </c>
-      <c r="O282" s="17" t="s">
-        <v>845</v>
+        <v>841</v>
+      </c>
+      <c r="O282" s="3" t="s">
+        <v>842</v>
       </c>
     </row>
     <row r="283" spans="1:15">
       <c r="A283" s="3" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B283" s="7"/>
       <c r="M283" s="3" t="s">
@@ -22618,19 +22629,19 @@
     </row>
     <row r="284" spans="1:15">
       <c r="A284" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B284" s="7"/>
       <c r="M284" s="3" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="O284" s="17" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
     </row>
     <row r="285" spans="1:15">
       <c r="A285" s="3" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="B285" s="7"/>
       <c r="M285" s="3" t="s">
@@ -22642,791 +22653,803 @@
     </row>
     <row r="286" spans="1:15">
       <c r="A286" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B286" s="7"/>
       <c r="M286" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="O286" s="17" t="s">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="287" spans="1:15">
+      <c r="A287" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="B287" s="7"/>
+      <c r="M287" s="3" t="s">
         <v>852</v>
       </c>
-      <c r="O286" s="17" t="s">
+      <c r="O287" s="17" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="287" spans="1:15">
-      <c r="B287" s="7"/>
-      <c r="O287" s="17"/>
-    </row>
     <row r="288" spans="1:15">
-      <c r="A288" t="s">
-        <v>5039</v>
-      </c>
-      <c r="M288" s="19" t="s">
-        <v>5040</v>
-      </c>
+      <c r="B288" s="7"/>
+      <c r="O288" s="17"/>
     </row>
     <row r="289" spans="1:15">
       <c r="A289" t="s">
-        <v>5041</v>
+        <v>5039</v>
       </c>
       <c r="M289" s="19" t="s">
-        <v>5042</v>
+        <v>5040</v>
       </c>
     </row>
     <row r="290" spans="1:15">
       <c r="A290" t="s">
-        <v>5043</v>
+        <v>5041</v>
       </c>
       <c r="M290" s="19" t="s">
-        <v>5044</v>
+        <v>5042</v>
       </c>
     </row>
     <row r="291" spans="1:15">
       <c r="A291" t="s">
-        <v>5045</v>
+        <v>5043</v>
       </c>
       <c r="M291" s="19" t="s">
-        <v>5051</v>
+        <v>5044</v>
       </c>
     </row>
     <row r="292" spans="1:15">
       <c r="A292" t="s">
-        <v>5046</v>
+        <v>5045</v>
       </c>
       <c r="M292" s="19" t="s">
-        <v>5052</v>
+        <v>5051</v>
       </c>
     </row>
     <row r="293" spans="1:15">
       <c r="A293" t="s">
-        <v>5047</v>
+        <v>5046</v>
       </c>
       <c r="M293" s="19" t="s">
-        <v>5048</v>
+        <v>5052</v>
       </c>
     </row>
     <row r="294" spans="1:15">
       <c r="A294" t="s">
+        <v>5047</v>
+      </c>
+      <c r="M294" s="19" t="s">
+        <v>5048</v>
+      </c>
+    </row>
+    <row r="295" spans="1:15">
+      <c r="A295" t="s">
         <v>5049</v>
       </c>
-      <c r="M294" s="19" t="s">
+      <c r="M295" s="19" t="s">
         <v>5050</v>
-      </c>
-    </row>
-    <row r="296" spans="1:15">
-      <c r="A296" t="s">
-        <v>854</v>
-      </c>
-      <c r="B296" s="7" t="s">
-        <v>855</v>
-      </c>
-      <c r="M296" t="s">
-        <v>856</v>
-      </c>
-      <c r="O296" s="17" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="297" spans="1:15">
       <c r="A297" t="s">
+        <v>854</v>
+      </c>
+      <c r="B297" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="M297" t="s">
+        <v>856</v>
+      </c>
+      <c r="O297" s="17" t="s">
+        <v>857</v>
+      </c>
+    </row>
+    <row r="298" spans="1:15">
+      <c r="A298" t="s">
         <v>858</v>
       </c>
-      <c r="B297" s="7" t="s">
+      <c r="B298" s="7" t="s">
         <v>859</v>
       </c>
-      <c r="M297" t="s">
+      <c r="M298" t="s">
         <v>860</v>
       </c>
-      <c r="O297" s="17" t="s">
+      <c r="O298" s="17" t="s">
         <v>861</v>
-      </c>
-    </row>
-    <row r="299" spans="1:15">
-      <c r="A299" t="s">
-        <v>862</v>
-      </c>
-      <c r="B299" s="7" t="s">
-        <v>862</v>
-      </c>
-      <c r="M299" t="s">
-        <v>863</v>
-      </c>
-      <c r="O299" s="17" t="s">
-        <v>863</v>
       </c>
     </row>
     <row r="300" spans="1:15">
       <c r="A300" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="B300" s="7" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="M300" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="O300" s="17" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="301" spans="1:15">
       <c r="A301" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="B301" s="7" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="M301" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="O301" s="17" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="302" spans="1:15">
       <c r="A302" t="s">
+        <v>866</v>
+      </c>
+      <c r="B302" s="7" t="s">
+        <v>866</v>
+      </c>
+      <c r="M302" t="s">
+        <v>867</v>
+      </c>
+      <c r="O302" s="17" t="s">
+        <v>867</v>
+      </c>
+    </row>
+    <row r="303" spans="1:15">
+      <c r="A303" t="s">
         <v>868</v>
       </c>
-      <c r="B302" s="7" t="s">
+      <c r="B303" s="7" t="s">
         <v>868</v>
       </c>
-      <c r="M302" t="s">
+      <c r="M303" t="s">
         <v>869</v>
       </c>
-      <c r="O302" s="17" t="s">
+      <c r="O303" s="17" t="s">
         <v>869</v>
-      </c>
-    </row>
-    <row r="304" spans="1:15">
-      <c r="A304" t="s">
-        <v>870</v>
-      </c>
-      <c r="B304" s="3" t="s">
-        <v>871</v>
-      </c>
-      <c r="M304" t="s">
-        <v>872</v>
-      </c>
-      <c r="O304" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="305" spans="1:15">
       <c r="A305" t="s">
+        <v>870</v>
+      </c>
+      <c r="B305" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="M305" t="s">
+        <v>872</v>
+      </c>
+      <c r="O305" t="s">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="306" spans="1:15">
+      <c r="A306" t="s">
         <v>874</v>
       </c>
-      <c r="B305" s="3" t="s">
+      <c r="B306" s="3" t="s">
         <v>875</v>
       </c>
-      <c r="M305" t="s">
+      <c r="M306" t="s">
         <v>876</v>
       </c>
-      <c r="O305" t="s">
+      <c r="O306" t="s">
         <v>877</v>
-      </c>
-    </row>
-    <row r="307" spans="1:15">
-      <c r="A307" t="s">
-        <v>878</v>
-      </c>
-      <c r="B307" s="3" t="s">
-        <v>879</v>
-      </c>
-      <c r="M307" t="s">
-        <v>880</v>
-      </c>
-      <c r="O307" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="308" spans="1:15">
       <c r="A308" t="s">
-        <v>882</v>
+        <v>878</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>883</v>
+        <v>879</v>
       </c>
       <c r="M308" t="s">
-        <v>884</v>
+        <v>880</v>
       </c>
       <c r="O308" t="s">
-        <v>885</v>
+        <v>881</v>
       </c>
     </row>
     <row r="309" spans="1:15">
       <c r="A309" t="s">
+        <v>882</v>
+      </c>
+      <c r="B309" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="M309" t="s">
+        <v>884</v>
+      </c>
+      <c r="O309" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="310" spans="1:15">
+      <c r="A310" t="s">
         <v>886</v>
       </c>
-      <c r="B309" s="3" t="s">
+      <c r="B310" s="3" t="s">
         <v>887</v>
       </c>
-      <c r="M309" t="s">
+      <c r="M310" t="s">
         <v>888</v>
       </c>
-      <c r="O309" t="s">
+      <c r="O310" t="s">
         <v>889</v>
-      </c>
-    </row>
-    <row r="311" spans="1:15">
-      <c r="A311" t="s">
-        <v>890</v>
-      </c>
-      <c r="B311" t="s">
-        <v>891</v>
-      </c>
-      <c r="C311" t="s">
-        <v>891</v>
-      </c>
-      <c r="D311" t="s">
-        <v>891</v>
-      </c>
-      <c r="E311" t="s">
-        <v>891</v>
-      </c>
-      <c r="F311" t="s">
-        <v>891</v>
-      </c>
-      <c r="G311" t="s">
-        <v>891</v>
-      </c>
-      <c r="H311" t="s">
-        <v>891</v>
-      </c>
-      <c r="I311" t="s">
-        <v>891</v>
-      </c>
-      <c r="J311" t="s">
-        <v>891</v>
-      </c>
-      <c r="K311" t="s">
-        <v>891</v>
-      </c>
-      <c r="L311" t="s">
-        <v>891</v>
-      </c>
-      <c r="M311" t="s">
-        <v>891</v>
-      </c>
-      <c r="N311" t="s">
-        <v>891</v>
-      </c>
-      <c r="O311" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="312" spans="1:15">
       <c r="A312" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="B312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="C312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="D312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="E312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="F312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="G312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="H312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="I312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="J312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="L312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="M312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="N312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="O312" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
     </row>
     <row r="313" spans="1:15">
       <c r="A313" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="B313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="D313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="F313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="G313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="H313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="I313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="J313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="K313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="L313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="M313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="N313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="O313" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="314" spans="1:15">
       <c r="A314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="D314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="F314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="G314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="H314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="I314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="J314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="K314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="L314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="M314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="N314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="O314" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="315" spans="1:15">
       <c r="A315" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="D315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="E315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="F315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="G315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="H315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="I315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="J315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="L315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="M315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="N315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="O315" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="316" spans="1:15">
       <c r="A316" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="B316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="D316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="E316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="G316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="H316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="I316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="J316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="K316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="L316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="M316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="N316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="O316" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
     <row r="317" spans="1:15">
       <c r="A317" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="B317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="D317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="F317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="H317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="J317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="K317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="L317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="M317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="N317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="O317" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="318" spans="1:15">
       <c r="A318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="D318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="F318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="H318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="I318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="J318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="K318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="L318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="M318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="N318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="O318" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="319" spans="1:15">
       <c r="A319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="D319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="F319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="G319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="H319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="I319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="J319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="K319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="L319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="M319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="N319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="O319" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="320" spans="1:15">
       <c r="A320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="D320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="F320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="G320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="H320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="I320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="J320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="K320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="L320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="M320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="N320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="O320" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="321" spans="1:15">
       <c r="A321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="D321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="F321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="I321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="J321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="K321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="L321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="M321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="N321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="O321" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="322" spans="1:15">
       <c r="A322" t="s">
+        <v>904</v>
+      </c>
+      <c r="B322" t="s">
+        <v>904</v>
+      </c>
+      <c r="C322" t="s">
+        <v>904</v>
+      </c>
+      <c r="D322" t="s">
+        <v>904</v>
+      </c>
+      <c r="E322" t="s">
+        <v>904</v>
+      </c>
+      <c r="F322" t="s">
+        <v>904</v>
+      </c>
+      <c r="G322" t="s">
+        <v>904</v>
+      </c>
+      <c r="H322" t="s">
+        <v>904</v>
+      </c>
+      <c r="I322" t="s">
+        <v>904</v>
+      </c>
+      <c r="J322" t="s">
+        <v>904</v>
+      </c>
+      <c r="K322" t="s">
+        <v>904</v>
+      </c>
+      <c r="L322" t="s">
+        <v>904</v>
+      </c>
+      <c r="M322" t="s">
+        <v>904</v>
+      </c>
+      <c r="N322" t="s">
+        <v>904</v>
+      </c>
+      <c r="O322" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="323" spans="1:15">
+      <c r="A323" t="s">
         <v>905</v>
       </c>
-      <c r="B322" t="s">
+      <c r="B323" t="s">
         <v>905</v>
       </c>
-      <c r="C322" t="s">
+      <c r="C323" t="s">
         <v>905</v>
       </c>
-      <c r="D322" t="s">
+      <c r="D323" t="s">
         <v>905</v>
       </c>
-      <c r="E322" t="s">
+      <c r="E323" t="s">
         <v>905</v>
       </c>
-      <c r="F322" t="s">
+      <c r="F323" t="s">
         <v>905</v>
       </c>
-      <c r="G322" t="s">
+      <c r="G323" t="s">
         <v>905</v>
       </c>
-      <c r="H322" t="s">
+      <c r="H323" t="s">
         <v>905</v>
       </c>
-      <c r="I322" t="s">
+      <c r="I323" t="s">
         <v>905</v>
       </c>
-      <c r="J322" t="s">
+      <c r="J323" t="s">
         <v>905</v>
       </c>
-      <c r="K322" t="s">
+      <c r="K323" t="s">
         <v>905</v>
       </c>
-      <c r="L322" t="s">
+      <c r="L323" t="s">
         <v>905</v>
       </c>
-      <c r="M322" t="s">
+      <c r="M323" t="s">
         <v>905</v>
       </c>
-      <c r="N322" t="s">
+      <c r="N323" t="s">
         <v>905</v>
       </c>
-      <c r="O322" t="s">
+      <c r="O323" t="s">
         <v>905</v>
       </c>
     </row>
@@ -28342,7 +28365,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q487"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A486" workbookViewId="0">
+    <sheetView topLeftCell="A486" workbookViewId="0">
       <selection activeCell="D486" sqref="D486"/>
     </sheetView>
   </sheetViews>

</xml_diff>